<commit_message>
Annual summary now adds expenses
</commit_message>
<xml_diff>
--- a/Lava3.TestFiles/TestFiles/Test.xlsx
+++ b/Lava3.TestFiles/TestFiles/Test.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="510" yWindow="585" windowWidth="15555" windowHeight="13155" tabRatio="554"/>
+    <workbookView xWindow="510" yWindow="585" windowWidth="15555" windowHeight="13155" tabRatio="554" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Annual Summary" sheetId="2" r:id="rId1"/>
@@ -2010,7 +2010,7 @@
     <xf numFmtId="0" fontId="44" fillId="0" borderId="13"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="150">
+  <cellXfs count="147">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="44" fontId="19" fillId="0" borderId="0" xfId="756" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="20" fillId="0" borderId="0" xfId="801" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -2068,8 +2068,6 @@
     </xf>
     <xf numFmtId="164" fontId="27" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="18" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="802" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="28" fillId="0" borderId="0" xfId="801" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="28" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -2214,13 +2212,12 @@
     </xf>
     <xf numFmtId="8" fontId="19" fillId="0" borderId="0" xfId="756" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="164" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -3546,9 +3543,9 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:AB75"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" workbookViewId="0">
+    <sheetView zoomScale="80" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B20" sqref="B20"/>
+      <selection pane="bottomLeft" activeCell="D38" sqref="D38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.625" defaultRowHeight="12"/>
@@ -3571,10 +3568,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:25" ht="12.75">
-      <c r="A1" s="83" t="s">
+      <c r="A1" s="81" t="s">
         <v>95</v>
       </c>
-      <c r="B1" s="83"/>
+      <c r="B1" s="81"/>
       <c r="D1" s="21"/>
       <c r="E1" s="21"/>
       <c r="F1" s="21"/>
@@ -3630,11 +3627,11 @@
       <c r="E3" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="F3" s="140" t="s">
+      <c r="F3" s="137" t="s">
         <v>50</v>
       </c>
-      <c r="G3" s="140"/>
-      <c r="H3" s="140"/>
+      <c r="G3" s="137"/>
+      <c r="H3" s="137"/>
       <c r="I3" s="11"/>
       <c r="J3" s="11"/>
       <c r="K3" s="23"/>
@@ -3653,17 +3650,17 @@
       <c r="X3" s="22"/>
       <c r="Y3" s="22"/>
     </row>
-    <row r="4" spans="1:25" s="108" customFormat="1" ht="12.75">
-      <c r="A4" s="63" t="s">
+    <row r="4" spans="1:25" s="106" customFormat="1" ht="12.75">
+      <c r="A4" s="61" t="s">
         <v>27</v>
       </c>
       <c r="B4" s="33" t="s">
         <v>51</v>
       </c>
-      <c r="C4" s="62" t="s">
+      <c r="C4" s="60" t="s">
         <v>52</v>
       </c>
-      <c r="D4" s="62" t="s">
+      <c r="D4" s="60" t="s">
         <v>53</v>
       </c>
       <c r="E4" s="34" t="s">
@@ -3678,7 +3675,7 @@
       <c r="H4" s="34" t="s">
         <v>9</v>
       </c>
-      <c r="I4" s="62" t="s">
+      <c r="I4" s="60" t="s">
         <v>12</v>
       </c>
       <c r="J4" s="25"/>
@@ -3697,16 +3694,16 @@
       <c r="W4" s="22"/>
       <c r="X4" s="22"/>
     </row>
-    <row r="5" spans="1:25" s="109" customFormat="1" ht="12.75">
-      <c r="A5" s="111"/>
-      <c r="B5" s="61"/>
-      <c r="C5" s="112"/>
-      <c r="D5" s="112"/>
+    <row r="5" spans="1:25" s="107" customFormat="1" ht="12.75">
+      <c r="A5" s="109"/>
+      <c r="B5" s="59"/>
+      <c r="C5" s="110"/>
+      <c r="D5" s="110"/>
       <c r="E5" s="25"/>
       <c r="F5" s="25"/>
       <c r="G5" s="25"/>
       <c r="H5" s="25"/>
-      <c r="I5" s="110"/>
+      <c r="I5" s="108"/>
       <c r="J5" s="25"/>
       <c r="K5" s="25"/>
       <c r="L5" s="25"/>
@@ -3723,36 +3720,36 @@
       <c r="W5" s="22"/>
       <c r="X5" s="22"/>
     </row>
-    <row r="6" spans="1:25" s="109" customFormat="1" ht="12.75">
-      <c r="A6" s="65"/>
-      <c r="B6" s="66" t="s">
+    <row r="6" spans="1:25" s="107" customFormat="1" ht="12.75">
+      <c r="A6" s="63"/>
+      <c r="B6" s="64" t="s">
         <v>55</v>
       </c>
-      <c r="C6" s="113">
+      <c r="C6" s="111">
         <f t="shared" ref="C6:I6" si="0">SUM(C5:C5)</f>
         <v>0</v>
       </c>
-      <c r="D6" s="113">
+      <c r="D6" s="111">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E6" s="113">
+      <c r="E6" s="111">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="F6" s="113">
+      <c r="F6" s="111">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G6" s="113">
+      <c r="G6" s="111">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H6" s="113">
+      <c r="H6" s="111">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I6" s="113">
+      <c r="I6" s="111">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -3772,16 +3769,16 @@
       <c r="W6" s="22"/>
       <c r="X6" s="22"/>
     </row>
-    <row r="7" spans="1:25" s="109" customFormat="1" ht="12.75">
-      <c r="A7" s="105"/>
-      <c r="B7" s="61"/>
-      <c r="C7" s="110"/>
-      <c r="D7" s="110"/>
+    <row r="7" spans="1:25" s="107" customFormat="1" ht="12.75">
+      <c r="A7" s="103"/>
+      <c r="B7" s="59"/>
+      <c r="C7" s="108"/>
+      <c r="D7" s="108"/>
       <c r="E7" s="25"/>
       <c r="F7" s="25"/>
       <c r="G7" s="25"/>
       <c r="H7" s="25"/>
-      <c r="I7" s="110"/>
+      <c r="I7" s="108"/>
       <c r="J7" s="25"/>
       <c r="K7" s="25"/>
       <c r="L7" s="25"/>
@@ -3798,16 +3795,16 @@
       <c r="W7" s="22"/>
       <c r="X7" s="22"/>
     </row>
-    <row r="8" spans="1:25" s="59" customFormat="1" ht="12.75">
-      <c r="A8" s="60"/>
-      <c r="B8" s="61"/>
-      <c r="C8" s="55"/>
-      <c r="D8" s="55"/>
+    <row r="8" spans="1:25" s="57" customFormat="1" ht="12.75">
+      <c r="A8" s="58"/>
+      <c r="B8" s="59"/>
+      <c r="C8" s="53"/>
+      <c r="D8" s="53"/>
       <c r="E8" s="25"/>
       <c r="F8" s="25"/>
       <c r="G8" s="25"/>
       <c r="H8" s="25"/>
-      <c r="I8" s="55"/>
+      <c r="I8" s="53"/>
       <c r="J8" s="25"/>
       <c r="K8" s="25"/>
       <c r="L8" s="25"/>
@@ -3824,7 +3821,7 @@
       <c r="W8" s="22"/>
       <c r="X8" s="22"/>
     </row>
-    <row r="9" spans="1:25" s="54" customFormat="1" ht="12.75">
+    <row r="9" spans="1:25" s="52" customFormat="1" ht="12.75">
       <c r="C9" s="21"/>
       <c r="D9" s="25"/>
       <c r="E9" s="25"/>
@@ -3873,10 +3870,10 @@
       <c r="X10" s="22"/>
     </row>
     <row r="11" spans="1:25" ht="12.75">
-      <c r="A11" s="137" t="s">
+      <c r="A11" s="136" t="s">
         <v>56</v>
       </c>
-      <c r="B11" s="137"/>
+      <c r="B11" s="136"/>
       <c r="D11" s="21"/>
       <c r="E11" s="21"/>
       <c r="F11" s="21"/>
@@ -3901,9 +3898,6 @@
     </row>
     <row r="12" spans="1:25" ht="12.75" customHeight="1">
       <c r="C12" s="21"/>
-      <c r="D12" s="138" t="s">
-        <v>57</v>
-      </c>
       <c r="E12" s="32" t="s">
         <v>49</v>
       </c>
@@ -3923,23 +3917,25 @@
       <c r="V12" s="22"/>
     </row>
     <row r="13" spans="1:25" ht="25.5">
-      <c r="A13" s="136" t="s">
+      <c r="A13" s="134" t="s">
         <v>27</v>
       </c>
-      <c r="B13" s="136" t="s">
+      <c r="B13" s="134" t="s">
         <v>0</v>
       </c>
       <c r="C13" s="24" t="s">
         <v>58</v>
       </c>
-      <c r="D13" s="139"/>
+      <c r="D13" s="135" t="s">
+        <v>57</v>
+      </c>
       <c r="E13" s="32" t="s">
         <v>59</v>
       </c>
       <c r="F13" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="G13" s="131" t="s">
+      <c r="G13" s="129" t="s">
         <v>113</v>
       </c>
       <c r="H13" s="11"/>
@@ -3959,7 +3955,7 @@
       <c r="A14" s="5">
         <v>42491</v>
       </c>
-      <c r="B14" s="80" t="s">
+      <c r="B14" s="78" t="s">
         <v>112</v>
       </c>
       <c r="C14" s="1">
@@ -3987,13 +3983,13 @@
       <c r="V14" s="22"/>
     </row>
     <row r="15" spans="1:25" ht="12.75">
-      <c r="A15" s="81">
+      <c r="A15" s="79">
         <v>42492</v>
       </c>
       <c r="B15" s="15" t="s">
         <v>114</v>
       </c>
-      <c r="C15" s="135">
+      <c r="C15" s="133">
         <v>20.45</v>
       </c>
       <c r="D15" s="21"/>
@@ -4018,7 +4014,7 @@
       <c r="V15" s="22"/>
     </row>
     <row r="16" spans="1:25" ht="12.75">
-      <c r="A16" s="84"/>
+      <c r="A16" s="82"/>
       <c r="B16" s="15"/>
       <c r="C16" s="1"/>
       <c r="D16" s="21"/>
@@ -4041,7 +4037,7 @@
       <c r="V16" s="22"/>
     </row>
     <row r="17" spans="1:28" ht="12.75">
-      <c r="A17" s="85"/>
+      <c r="A17" s="83"/>
       <c r="B17" s="15"/>
       <c r="C17" s="1"/>
       <c r="D17" s="21"/>
@@ -4158,8 +4154,8 @@
       <c r="X20" s="22"/>
     </row>
     <row r="21" spans="1:28" ht="12.75">
-      <c r="A21" s="137"/>
-      <c r="B21" s="137"/>
+      <c r="A21" s="136"/>
+      <c r="B21" s="136"/>
       <c r="C21" s="3"/>
       <c r="G21" s="21"/>
       <c r="H21" s="21"/>
@@ -4182,10 +4178,10 @@
       <c r="Y21" s="22"/>
     </row>
     <row r="22" spans="1:28" ht="12.75" customHeight="1">
-      <c r="A22" s="44" t="s">
+      <c r="A22" s="42" t="s">
         <v>60</v>
       </c>
-      <c r="F22" s="76"/>
+      <c r="F22" s="74"/>
       <c r="I22" s="3"/>
       <c r="J22" s="21"/>
       <c r="K22" s="27"/>
@@ -4205,34 +4201,34 @@
     </row>
     <row r="23" spans="1:28" ht="12.75" customHeight="1">
       <c r="A23" s="4"/>
-      <c r="B23" s="90" t="s">
+      <c r="B23" s="88" t="s">
         <v>61</v>
       </c>
-      <c r="C23" s="91" t="s">
+      <c r="C23" s="89" t="s">
         <v>62</v>
       </c>
-      <c r="D23" s="91" t="s">
+      <c r="D23" s="89" t="s">
         <v>63</v>
       </c>
-      <c r="E23" s="91" t="s">
+      <c r="E23" s="89" t="s">
         <v>64</v>
       </c>
-      <c r="F23" s="91" t="s">
+      <c r="F23" s="89" t="s">
         <v>65</v>
       </c>
-      <c r="G23" s="91" t="s">
+      <c r="G23" s="89" t="s">
         <v>66</v>
       </c>
-      <c r="H23" s="91" t="s">
+      <c r="H23" s="89" t="s">
         <v>67</v>
       </c>
-      <c r="I23" s="91" t="s">
+      <c r="I23" s="89" t="s">
         <v>68</v>
       </c>
-      <c r="J23" s="91" t="s">
+      <c r="J23" s="89" t="s">
         <v>110</v>
       </c>
-      <c r="K23" s="132" t="s">
+      <c r="K23" s="130" t="s">
         <v>111</v>
       </c>
       <c r="N23" s="11"/>
@@ -4253,35 +4249,35 @@
     </row>
     <row r="24" spans="1:28" ht="12.75">
       <c r="A24" s="19"/>
-      <c r="B24" s="90" t="s">
+      <c r="B24" s="88" t="s">
         <v>106</v>
       </c>
-      <c r="C24" s="125" t="s">
+      <c r="C24" s="123" t="s">
         <v>107</v>
       </c>
-      <c r="D24" s="133">
+      <c r="D24" s="131">
         <v>42370</v>
       </c>
-      <c r="E24" s="133">
+      <c r="E24" s="131">
         <v>42401</v>
       </c>
-      <c r="F24" s="91">
+      <c r="F24" s="89">
         <f>30</f>
         <v>30</v>
       </c>
-      <c r="G24" s="91">
+      <c r="G24" s="89">
         <v>7.5</v>
       </c>
-      <c r="H24" s="91">
+      <c r="H24" s="89">
         <v>1</v>
       </c>
-      <c r="I24" s="91">
+      <c r="I24" s="89">
         <v>500</v>
       </c>
-      <c r="J24" s="91">
+      <c r="J24" s="89">
         <v>500</v>
       </c>
-      <c r="K24" s="132">
+      <c r="K24" s="130">
         <v>500</v>
       </c>
       <c r="L24" s="22"/>
@@ -4301,30 +4297,30 @@
       <c r="AA24" s="22"/>
       <c r="AB24" s="22"/>
     </row>
-    <row r="25" spans="1:28" s="108" customFormat="1" ht="15.75">
-      <c r="A25" s="106"/>
-      <c r="B25" s="134" t="s">
+    <row r="25" spans="1:28" s="106" customFormat="1" ht="15.75">
+      <c r="A25" s="104"/>
+      <c r="B25" s="132" t="s">
         <v>108</v>
       </c>
-      <c r="C25" s="125" t="s">
+      <c r="C25" s="123" t="s">
         <v>109</v>
       </c>
-      <c r="D25" s="133">
+      <c r="D25" s="131">
         <v>42401</v>
       </c>
-      <c r="E25" s="133"/>
-      <c r="F25" s="91"/>
-      <c r="G25" s="91">
+      <c r="E25" s="131"/>
+      <c r="F25" s="89"/>
+      <c r="G25" s="89">
         <v>15</v>
       </c>
-      <c r="H25" s="91">
+      <c r="H25" s="89">
         <v>1</v>
       </c>
-      <c r="I25" s="91">
+      <c r="I25" s="89">
         <v>1000</v>
       </c>
-      <c r="J25" s="91"/>
-      <c r="K25" s="132"/>
+      <c r="J25" s="89"/>
+      <c r="K25" s="130"/>
       <c r="L25" s="22"/>
       <c r="M25" s="22"/>
       <c r="O25" s="22"/>
@@ -4342,13 +4338,13 @@
       <c r="AA25" s="22"/>
       <c r="AB25" s="22"/>
     </row>
-    <row r="26" spans="1:28" s="78" customFormat="1" ht="15.75">
-      <c r="A26" s="79"/>
-      <c r="B26" s="89"/>
-      <c r="C26" s="88"/>
-      <c r="D26" s="106"/>
-      <c r="E26" s="106"/>
-      <c r="F26" s="92"/>
+    <row r="26" spans="1:28" s="76" customFormat="1" ht="15.75">
+      <c r="A26" s="77"/>
+      <c r="B26" s="87"/>
+      <c r="C26" s="86"/>
+      <c r="D26" s="104"/>
+      <c r="E26" s="104"/>
+      <c r="F26" s="90"/>
       <c r="G26" s="4"/>
       <c r="H26" s="13"/>
       <c r="I26" s="12"/>
@@ -4383,7 +4379,7 @@
         <f>SUM(G24:G26)</f>
         <v>22.5</v>
       </c>
-      <c r="H27" s="75">
+      <c r="H27" s="73">
         <f>SUM(H24:H26)</f>
         <v>2</v>
       </c>
@@ -4413,7 +4409,7 @@
         <f>H27/275</f>
         <v>7.2727272727272727E-3</v>
       </c>
-      <c r="I28" s="77" t="s">
+      <c r="I28" s="75" t="s">
         <v>69</v>
       </c>
       <c r="J28" s="22"/>
@@ -4436,8 +4432,8 @@
       <c r="C31" s="9"/>
     </row>
     <row r="33" spans="1:8" ht="12.75">
-      <c r="B33" s="73"/>
-      <c r="C33" s="73"/>
+      <c r="B33" s="71"/>
+      <c r="C33" s="71"/>
       <c r="E33" s="22"/>
       <c r="F33" s="22"/>
       <c r="G33" s="22"/>
@@ -4841,9 +4837,8 @@
     <sortCondition ref="B5"/>
     <sortCondition ref="A5"/>
   </sortState>
-  <mergeCells count="4">
+  <mergeCells count="3">
     <mergeCell ref="A11:B11"/>
-    <mergeCell ref="D12:D13"/>
     <mergeCell ref="A21:B21"/>
     <mergeCell ref="F3:H3"/>
   </mergeCells>
@@ -4863,7 +4858,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B26" sqref="B26"/>
+      <selection pane="bottomLeft" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12"/>
@@ -4872,7 +4867,7 @@
     <col min="2" max="2" width="53.125" customWidth="1"/>
     <col min="3" max="3" width="14" customWidth="1"/>
     <col min="4" max="4" width="14.375" customWidth="1"/>
-    <col min="5" max="5" width="13" style="38" customWidth="1"/>
+    <col min="5" max="5" width="13" style="36" customWidth="1"/>
     <col min="6" max="6" width="12.125" customWidth="1"/>
     <col min="7" max="7" width="24.875" customWidth="1"/>
     <col min="8" max="8" width="42.75" customWidth="1"/>
@@ -4882,23 +4877,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
-      <c r="A1" s="42"/>
-      <c r="B1" s="42"/>
-      <c r="C1" s="42"/>
-      <c r="D1" s="42"/>
-      <c r="E1" s="42"/>
-      <c r="F1" s="141" t="s">
+      <c r="A1" s="40"/>
+      <c r="B1" s="40"/>
+      <c r="C1" s="40"/>
+      <c r="D1" s="40"/>
+      <c r="E1" s="40"/>
+      <c r="F1" s="138" t="s">
         <v>26</v>
       </c>
-      <c r="G1" s="141"/>
+      <c r="G1" s="138"/>
       <c r="H1" s="20"/>
       <c r="I1" s="20"/>
     </row>
     <row r="2" spans="1:9">
-      <c r="A2" s="42" t="s">
+      <c r="A2" s="40" t="s">
         <v>27</v>
       </c>
-      <c r="B2" s="42" t="s">
+      <c r="B2" s="40" t="s">
         <v>0</v>
       </c>
       <c r="C2" s="20" t="s">
@@ -4916,141 +4911,141 @@
       <c r="G2" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="H2" s="43" t="s">
+      <c r="H2" s="41" t="s">
         <v>32</v>
       </c>
       <c r="I2" s="20" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:9" s="122" customFormat="1" ht="14.25" customHeight="1">
-      <c r="A3" s="123">
+    <row r="3" spans="1:9" s="120" customFormat="1" ht="14.25" customHeight="1">
+      <c r="A3" s="121">
         <v>42466</v>
       </c>
-      <c r="B3" s="122" t="s">
+      <c r="B3" s="120" t="s">
         <v>33</v>
       </c>
-      <c r="G3" s="122">
+      <c r="G3" s="120">
         <v>100</v>
       </c>
     </row>
-    <row r="4" spans="1:9" s="122" customFormat="1" ht="15">
-      <c r="A4" s="123">
+    <row r="4" spans="1:9" s="120" customFormat="1" ht="15">
+      <c r="A4" s="121">
         <v>42468</v>
       </c>
-      <c r="B4" s="122" t="s">
+      <c r="B4" s="120" t="s">
         <v>34</v>
       </c>
-      <c r="C4" s="122">
+      <c r="C4" s="120">
         <v>23.62</v>
       </c>
-      <c r="D4" s="122">
+      <c r="D4" s="120">
         <v>0</v>
       </c>
-      <c r="E4" s="122">
+      <c r="E4" s="120">
         <v>76.38</v>
       </c>
-      <c r="F4" s="122">
+      <c r="F4" s="120">
         <v>-23.62</v>
       </c>
     </row>
-    <row r="5" spans="1:9" s="122" customFormat="1" ht="15">
-      <c r="A5" s="123">
+    <row r="5" spans="1:9" s="120" customFormat="1" ht="15">
+      <c r="A5" s="121">
         <v>42471</v>
       </c>
-      <c r="B5" s="122" t="s">
+      <c r="B5" s="120" t="s">
         <v>36</v>
       </c>
-      <c r="C5" s="122">
+      <c r="C5" s="120">
         <v>0.96</v>
       </c>
-      <c r="D5" s="122">
+      <c r="D5" s="120">
         <v>0</v>
       </c>
-      <c r="E5" s="122">
+      <c r="E5" s="120">
         <v>75.42</v>
       </c>
-      <c r="F5" s="122">
+      <c r="F5" s="120">
         <v>-24.580000000000002</v>
       </c>
     </row>
-    <row r="6" spans="1:9" s="121" customFormat="1" ht="15">
-      <c r="A6" s="124">
+    <row r="6" spans="1:9" s="119" customFormat="1" ht="15">
+      <c r="A6" s="122">
         <v>42609</v>
       </c>
-      <c r="B6" s="127" t="s">
+      <c r="B6" s="125" t="s">
         <v>88</v>
       </c>
-      <c r="C6" s="121">
+      <c r="C6" s="119">
         <v>3.1</v>
       </c>
-      <c r="D6" s="121">
+      <c r="D6" s="119">
         <v>0</v>
       </c>
-      <c r="E6" s="121">
+      <c r="E6" s="119">
         <v>72.320000000000007</v>
       </c>
-      <c r="F6" s="121">
+      <c r="F6" s="119">
         <v>-3.1</v>
       </c>
     </row>
-    <row r="7" spans="1:9" s="121" customFormat="1" ht="15">
-      <c r="A7" s="124">
+    <row r="7" spans="1:9" s="119" customFormat="1" ht="15">
+      <c r="A7" s="122">
         <v>42610</v>
       </c>
-      <c r="B7" s="121" t="s">
+      <c r="B7" s="119" t="s">
         <v>89</v>
       </c>
-      <c r="C7" s="121">
+      <c r="C7" s="119">
         <v>0</v>
       </c>
-      <c r="D7" s="121">
+      <c r="D7" s="119">
         <v>1000</v>
       </c>
-      <c r="E7" s="121">
+      <c r="E7" s="119">
         <v>1072.32</v>
       </c>
-      <c r="F7" s="121">
+      <c r="F7" s="119">
         <v>996.9</v>
       </c>
     </row>
-    <row r="8" spans="1:9" s="121" customFormat="1" ht="15">
-      <c r="A8" s="124">
+    <row r="8" spans="1:9" s="119" customFormat="1" ht="15">
+      <c r="A8" s="122">
         <v>42611</v>
       </c>
-      <c r="B8" s="121" t="s">
+      <c r="B8" s="119" t="s">
         <v>37</v>
       </c>
-      <c r="C8" s="121">
+      <c r="C8" s="119">
         <v>34.99</v>
       </c>
-      <c r="D8" s="121">
+      <c r="D8" s="119">
         <v>0</v>
       </c>
-      <c r="E8" s="121">
+      <c r="E8" s="119">
         <v>1037.33</v>
       </c>
-      <c r="F8" s="121">
+      <c r="F8" s="119">
         <v>961.91</v>
       </c>
     </row>
-    <row r="9" spans="1:9" s="121" customFormat="1" ht="15">
-      <c r="A9" s="124">
+    <row r="9" spans="1:9" s="119" customFormat="1" ht="15">
+      <c r="A9" s="122">
         <v>42612</v>
       </c>
-      <c r="B9" s="126" t="s">
+      <c r="B9" s="124" t="s">
         <v>96</v>
       </c>
-      <c r="C9" s="121">
+      <c r="C9" s="119">
         <v>14.5</v>
       </c>
-      <c r="D9" s="121">
+      <c r="D9" s="119">
         <v>0</v>
       </c>
-      <c r="E9" s="121">
+      <c r="E9" s="119">
         <v>1022.8299999999999</v>
       </c>
-      <c r="F9" s="121">
+      <c r="F9" s="119">
         <v>947.41</v>
       </c>
     </row>
@@ -5072,9 +5067,9 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:J61"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B3" sqref="B3"/>
+      <selection pane="bottomLeft" activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="12"/>
@@ -5085,393 +5080,393 @@
     <col min="4" max="4" width="45.375" style="2" customWidth="1"/>
     <col min="5" max="5" width="18.75" style="2" customWidth="1"/>
     <col min="6" max="6" width="34.25" style="2" customWidth="1"/>
-    <col min="7" max="7" width="11.75" style="71" customWidth="1"/>
-    <col min="8" max="8" width="11.625" style="71" customWidth="1"/>
+    <col min="7" max="7" width="11.75" style="69" customWidth="1"/>
+    <col min="8" max="8" width="11.625" style="69" customWidth="1"/>
     <col min="9" max="9" width="47" style="2" customWidth="1"/>
     <col min="10" max="10" width="28.75" style="2" customWidth="1"/>
     <col min="11" max="12" width="9" style="2" customWidth="1"/>
     <col min="13" max="16384" width="9" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15">
+    <row r="1" spans="1:10">
       <c r="A1" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="B1" s="36" t="s">
+      <c r="B1" s="92" t="s">
         <v>39</v>
       </c>
-      <c r="C1" s="35" t="s">
+      <c r="C1" s="92" t="s">
         <v>40</v>
       </c>
-      <c r="D1" s="35" t="s">
+      <c r="D1" s="92" t="s">
         <v>41</v>
       </c>
-      <c r="E1" s="35" t="s">
+      <c r="E1" s="92" t="s">
         <v>42</v>
       </c>
-      <c r="F1" s="35" t="s">
+      <c r="F1" s="92" t="s">
         <v>1</v>
       </c>
-      <c r="G1" s="35" t="s">
+      <c r="G1" s="92" t="s">
         <v>43</v>
       </c>
-      <c r="H1" s="71" t="s">
+      <c r="H1" s="92" t="s">
         <v>44</v>
       </c>
-      <c r="I1" s="35" t="s">
+      <c r="I1" s="92" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:10" s="71" customFormat="1" ht="15">
-      <c r="A2" s="111">
+    <row r="2" spans="1:10" s="69" customFormat="1" ht="15">
+      <c r="A2" s="109">
         <v>42611</v>
       </c>
-      <c r="B2" s="37">
+      <c r="B2" s="35">
         <v>42592</v>
       </c>
-      <c r="C2" s="111">
+      <c r="C2" s="109">
         <v>42524</v>
       </c>
-      <c r="D2" s="107" t="s">
+      <c r="D2" s="105" t="s">
         <v>45</v>
       </c>
-      <c r="E2" s="114">
+      <c r="E2" s="112">
         <v>-9</v>
       </c>
-      <c r="F2" s="116"/>
-      <c r="G2" s="71">
+      <c r="F2" s="114"/>
+      <c r="G2" s="69">
         <v>3</v>
       </c>
-      <c r="H2" s="71">
+      <c r="H2" s="69">
         <v>2</v>
       </c>
-      <c r="I2" s="70"/>
-      <c r="J2" s="69"/>
+      <c r="I2" s="68"/>
+      <c r="J2" s="67"/>
     </row>
     <row r="3" spans="1:10">
-      <c r="A3" s="111">
+      <c r="A3" s="109">
         <v>42611</v>
       </c>
-      <c r="B3" s="37"/>
-      <c r="C3" s="86">
+      <c r="B3" s="35"/>
+      <c r="C3" s="84">
         <v>42544</v>
       </c>
       <c r="D3" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="E3" s="58">
+      <c r="E3" s="56">
         <v>-13</v>
       </c>
-      <c r="F3" s="116"/>
-      <c r="I3" s="71"/>
-      <c r="J3" s="71"/>
+      <c r="F3" s="114"/>
+      <c r="I3" s="69"/>
+      <c r="J3" s="69"/>
     </row>
     <row r="4" spans="1:10">
-      <c r="A4" s="111">
+      <c r="A4" s="109">
         <v>42611</v>
       </c>
-      <c r="B4" s="37">
+      <c r="B4" s="35">
         <v>42592</v>
       </c>
-      <c r="C4" s="99">
+      <c r="C4" s="97">
         <v>42562</v>
       </c>
-      <c r="D4" s="119" t="s">
+      <c r="D4" s="117" t="s">
         <v>16</v>
       </c>
-      <c r="E4" s="58">
+      <c r="E4" s="56">
         <v>-11.99</v>
       </c>
-      <c r="F4" s="116"/>
-      <c r="I4" s="71"/>
-      <c r="J4" s="71"/>
+      <c r="F4" s="114"/>
+      <c r="I4" s="69"/>
+      <c r="J4" s="69"/>
     </row>
     <row r="5" spans="1:10">
-      <c r="A5" s="99"/>
-      <c r="B5" s="37"/>
-      <c r="C5" s="106">
+      <c r="A5" s="97"/>
+      <c r="B5" s="35"/>
+      <c r="C5" s="104">
         <v>42581</v>
       </c>
-      <c r="D5" s="120" t="s">
+      <c r="D5" s="118" t="s">
         <v>97</v>
       </c>
-      <c r="E5" s="58">
+      <c r="E5" s="56">
         <v>-22.15</v>
       </c>
-      <c r="F5" s="116"/>
-      <c r="G5" s="72">
+      <c r="F5" s="114"/>
+      <c r="G5" s="70">
         <v>4</v>
       </c>
-      <c r="H5" s="72">
+      <c r="H5" s="70">
         <v>5</v>
       </c>
-      <c r="I5" s="70"/>
-      <c r="J5" s="69"/>
+      <c r="I5" s="68"/>
+      <c r="J5" s="67"/>
     </row>
     <row r="6" spans="1:10">
-      <c r="A6" s="99"/>
-      <c r="B6" s="37"/>
-      <c r="C6" s="106">
+      <c r="A6" s="97"/>
+      <c r="B6" s="35"/>
+      <c r="C6" s="104">
         <v>42581</v>
       </c>
-      <c r="D6" s="120" t="s">
+      <c r="D6" s="118" t="s">
         <v>88</v>
       </c>
-      <c r="E6" s="58">
+      <c r="E6" s="56">
         <v>-0.66</v>
       </c>
-      <c r="F6" s="116"/>
-      <c r="G6" s="72"/>
-      <c r="H6" s="72"/>
-      <c r="I6" s="70"/>
-      <c r="J6" s="71"/>
+      <c r="F6" s="114"/>
+      <c r="G6" s="70"/>
+      <c r="H6" s="70"/>
+      <c r="I6" s="68"/>
+      <c r="J6" s="69"/>
     </row>
     <row r="7" spans="1:10">
-      <c r="A7" s="99"/>
-      <c r="B7" s="37"/>
-      <c r="C7" s="106">
+      <c r="A7" s="97"/>
+      <c r="B7" s="35"/>
+      <c r="C7" s="104">
         <v>42585</v>
       </c>
-      <c r="D7" s="120" t="s">
+      <c r="D7" s="118" t="s">
         <v>103</v>
       </c>
-      <c r="E7" s="58">
+      <c r="E7" s="56">
         <v>-6.85</v>
       </c>
-      <c r="F7" s="116"/>
-      <c r="G7" s="72"/>
-      <c r="H7" s="72"/>
-      <c r="I7" s="70"/>
-      <c r="J7" s="69"/>
+      <c r="F7" s="114"/>
+      <c r="G7" s="70"/>
+      <c r="H7" s="70"/>
+      <c r="I7" s="68"/>
+      <c r="J7" s="67"/>
     </row>
     <row r="8" spans="1:10">
-      <c r="B8" s="37"/>
-      <c r="C8" s="106">
+      <c r="B8" s="35"/>
+      <c r="C8" s="104">
         <v>42590</v>
       </c>
       <c r="D8" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="E8" s="58">
+      <c r="E8" s="56">
         <v>-25</v>
       </c>
-      <c r="F8" s="116"/>
+      <c r="F8" s="114"/>
     </row>
     <row r="9" spans="1:10">
-      <c r="B9" s="37"/>
-      <c r="C9" s="106">
+      <c r="B9" s="35"/>
+      <c r="C9" s="104">
         <v>42592</v>
       </c>
-      <c r="D9" s="120" t="s">
+      <c r="D9" s="118" t="s">
         <v>104</v>
       </c>
-      <c r="E9" s="58">
+      <c r="E9" s="56">
         <v>-174</v>
       </c>
-      <c r="F9" s="116"/>
+      <c r="F9" s="114"/>
     </row>
     <row r="10" spans="1:10">
-      <c r="B10" s="37"/>
-      <c r="C10" s="106">
+      <c r="B10" s="35"/>
+      <c r="C10" s="104">
         <v>42593</v>
       </c>
-      <c r="D10" s="120" t="s">
+      <c r="D10" s="118" t="s">
         <v>98</v>
       </c>
-      <c r="E10" s="58">
+      <c r="E10" s="56">
         <v>-35.020000000000003</v>
       </c>
-      <c r="F10" s="116"/>
+      <c r="F10" s="114"/>
     </row>
     <row r="11" spans="1:10">
-      <c r="B11" s="37"/>
-      <c r="C11" s="106">
+      <c r="B11" s="35"/>
+      <c r="C11" s="104">
         <v>42594</v>
       </c>
-      <c r="D11" s="120" t="s">
+      <c r="D11" s="118" t="s">
         <v>98</v>
       </c>
-      <c r="E11" s="58">
+      <c r="E11" s="56">
         <v>-11.99</v>
       </c>
-      <c r="F11" s="116"/>
+      <c r="F11" s="114"/>
     </row>
     <row r="12" spans="1:10">
-      <c r="A12" s="106"/>
-      <c r="B12" s="37"/>
-      <c r="C12" s="106"/>
+      <c r="A12" s="104"/>
+      <c r="B12" s="35"/>
+      <c r="C12" s="104"/>
       <c r="D12" s="8"/>
-      <c r="E12" s="58"/>
-      <c r="F12" s="116"/>
-      <c r="G12" s="72"/>
-      <c r="I12" s="70"/>
-      <c r="J12" s="108"/>
+      <c r="E12" s="56"/>
+      <c r="F12" s="114"/>
+      <c r="G12" s="70"/>
+      <c r="I12" s="68"/>
+      <c r="J12" s="106"/>
     </row>
     <row r="13" spans="1:10">
-      <c r="A13" s="106"/>
-      <c r="B13" s="37"/>
-      <c r="C13" s="106"/>
+      <c r="A13" s="104"/>
+      <c r="B13" s="35"/>
+      <c r="C13" s="104"/>
       <c r="D13" s="8"/>
-      <c r="E13" s="58"/>
-      <c r="F13" s="116"/>
-      <c r="I13" s="70"/>
+      <c r="E13" s="56"/>
+      <c r="F13" s="114"/>
+      <c r="I13" s="68"/>
     </row>
     <row r="14" spans="1:10">
-      <c r="B14" s="37"/>
-      <c r="C14" s="71"/>
-      <c r="D14" s="71"/>
-      <c r="E14" s="115"/>
-      <c r="F14" s="116"/>
+      <c r="B14" s="35"/>
+      <c r="C14" s="69"/>
+      <c r="D14" s="69"/>
+      <c r="E14" s="113"/>
+      <c r="F14" s="114"/>
     </row>
     <row r="15" spans="1:10">
-      <c r="B15" s="37"/>
-      <c r="E15" s="115"/>
-      <c r="F15" s="116"/>
+      <c r="B15" s="35"/>
+      <c r="E15" s="113"/>
+      <c r="F15" s="114"/>
     </row>
     <row r="16" spans="1:10">
-      <c r="E16" s="115"/>
-      <c r="F16" s="116"/>
+      <c r="E16" s="113"/>
+      <c r="F16" s="114"/>
     </row>
     <row r="17" spans="5:6">
-      <c r="E17" s="115"/>
-      <c r="F17" s="116"/>
+      <c r="E17" s="113"/>
+      <c r="F17" s="114"/>
     </row>
     <row r="18" spans="5:6">
-      <c r="E18" s="115"/>
-      <c r="F18" s="116"/>
+      <c r="E18" s="113"/>
+      <c r="F18" s="114"/>
     </row>
     <row r="19" spans="5:6">
-      <c r="E19" s="115"/>
-      <c r="F19" s="116"/>
+      <c r="E19" s="113"/>
+      <c r="F19" s="114"/>
     </row>
     <row r="20" spans="5:6">
-      <c r="E20" s="115"/>
-      <c r="F20" s="116"/>
+      <c r="E20" s="113"/>
+      <c r="F20" s="114"/>
     </row>
     <row r="21" spans="5:6">
-      <c r="E21" s="115"/>
-      <c r="F21" s="116"/>
+      <c r="E21" s="113"/>
+      <c r="F21" s="114"/>
     </row>
     <row r="22" spans="5:6">
-      <c r="E22" s="115"/>
-      <c r="F22" s="116"/>
+      <c r="E22" s="113"/>
+      <c r="F22" s="114"/>
     </row>
     <row r="23" spans="5:6">
-      <c r="E23" s="115"/>
+      <c r="E23" s="113"/>
     </row>
     <row r="24" spans="5:6">
-      <c r="E24" s="115"/>
+      <c r="E24" s="113"/>
     </row>
     <row r="25" spans="5:6">
-      <c r="E25" s="115"/>
+      <c r="E25" s="113"/>
     </row>
     <row r="26" spans="5:6">
-      <c r="E26" s="115"/>
+      <c r="E26" s="113"/>
     </row>
     <row r="27" spans="5:6">
-      <c r="E27" s="115"/>
+      <c r="E27" s="113"/>
     </row>
     <row r="28" spans="5:6">
-      <c r="E28" s="115"/>
+      <c r="E28" s="113"/>
     </row>
     <row r="29" spans="5:6">
-      <c r="E29" s="115"/>
+      <c r="E29" s="113"/>
     </row>
     <row r="30" spans="5:6">
-      <c r="E30" s="115"/>
+      <c r="E30" s="113"/>
     </row>
     <row r="31" spans="5:6">
-      <c r="E31" s="115"/>
+      <c r="E31" s="113"/>
     </row>
     <row r="32" spans="5:6">
-      <c r="E32" s="115"/>
+      <c r="E32" s="113"/>
     </row>
     <row r="33" spans="5:5">
-      <c r="E33" s="115"/>
+      <c r="E33" s="113"/>
     </row>
     <row r="34" spans="5:5">
-      <c r="E34" s="115"/>
+      <c r="E34" s="113"/>
     </row>
     <row r="35" spans="5:5">
-      <c r="E35" s="115"/>
+      <c r="E35" s="113"/>
     </row>
     <row r="36" spans="5:5">
-      <c r="E36" s="115"/>
+      <c r="E36" s="113"/>
     </row>
     <row r="37" spans="5:5">
-      <c r="E37" s="115"/>
+      <c r="E37" s="113"/>
     </row>
     <row r="38" spans="5:5">
-      <c r="E38" s="115"/>
+      <c r="E38" s="113"/>
     </row>
     <row r="39" spans="5:5">
-      <c r="E39" s="115"/>
+      <c r="E39" s="113"/>
     </row>
     <row r="40" spans="5:5">
-      <c r="E40" s="115"/>
+      <c r="E40" s="113"/>
     </row>
     <row r="41" spans="5:5">
-      <c r="E41" s="115"/>
+      <c r="E41" s="113"/>
     </row>
     <row r="42" spans="5:5">
-      <c r="E42" s="115"/>
+      <c r="E42" s="113"/>
     </row>
     <row r="43" spans="5:5">
-      <c r="E43" s="115"/>
+      <c r="E43" s="113"/>
     </row>
     <row r="44" spans="5:5">
-      <c r="E44" s="115"/>
+      <c r="E44" s="113"/>
     </row>
     <row r="45" spans="5:5">
-      <c r="E45" s="115"/>
+      <c r="E45" s="113"/>
     </row>
     <row r="46" spans="5:5">
-      <c r="E46" s="115"/>
+      <c r="E46" s="113"/>
     </row>
     <row r="47" spans="5:5">
-      <c r="E47" s="115"/>
+      <c r="E47" s="113"/>
     </row>
     <row r="48" spans="5:5">
-      <c r="E48" s="115"/>
+      <c r="E48" s="113"/>
     </row>
     <row r="49" spans="5:5">
-      <c r="E49" s="115"/>
+      <c r="E49" s="113"/>
     </row>
     <row r="50" spans="5:5">
-      <c r="E50" s="115"/>
+      <c r="E50" s="113"/>
     </row>
     <row r="51" spans="5:5">
-      <c r="E51" s="115"/>
+      <c r="E51" s="113"/>
     </row>
     <row r="52" spans="5:5">
-      <c r="E52" s="115"/>
+      <c r="E52" s="113"/>
     </row>
     <row r="53" spans="5:5">
-      <c r="E53" s="115"/>
+      <c r="E53" s="113"/>
     </row>
     <row r="54" spans="5:5">
-      <c r="E54" s="115"/>
+      <c r="E54" s="113"/>
     </row>
     <row r="55" spans="5:5">
-      <c r="E55" s="115"/>
+      <c r="E55" s="113"/>
     </row>
     <row r="56" spans="5:5">
-      <c r="E56" s="115"/>
+      <c r="E56" s="113"/>
     </row>
     <row r="57" spans="5:5">
-      <c r="E57" s="115"/>
+      <c r="E57" s="113"/>
     </row>
     <row r="58" spans="5:5">
-      <c r="E58" s="115"/>
+      <c r="E58" s="113"/>
     </row>
     <row r="59" spans="5:5">
-      <c r="E59" s="115"/>
+      <c r="E59" s="113"/>
     </row>
     <row r="60" spans="5:5">
-      <c r="E60" s="115"/>
+      <c r="E60" s="113"/>
     </row>
     <row r="61" spans="5:5">
-      <c r="E61" s="115"/>
+      <c r="E61" s="113"/>
     </row>
   </sheetData>
   <sortState ref="A2:J11">
@@ -5500,21 +5495,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
-      <c r="A1" s="40" t="s">
+      <c r="A1" s="38" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="40" t="s">
+      <c r="B1" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="40" t="s">
+      <c r="C1" s="38" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" s="39" customFormat="1">
-      <c r="A2" s="103" t="s">
+    <row r="2" spans="1:3" s="37" customFormat="1">
+      <c r="A2" s="101" t="s">
         <v>18</v>
       </c>
-      <c r="B2" s="103" t="s">
+      <c r="B2" s="101" t="s">
         <v>19</v>
       </c>
     </row>
@@ -5522,7 +5517,7 @@
       <c r="A3" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="B3" s="103" t="s">
+      <c r="B3" s="101" t="s">
         <v>21</v>
       </c>
     </row>
@@ -5530,64 +5525,64 @@
       <c r="A4" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="B4" s="67" t="s">
+      <c r="B4" s="65" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:3">
-      <c r="A5" s="100" t="s">
+      <c r="A5" s="98" t="s">
         <v>22</v>
       </c>
-      <c r="B5" s="101" t="s">
+      <c r="B5" s="99" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="6" spans="1:3">
-      <c r="A6" s="118" t="s">
+      <c r="A6" s="116" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="103" t="s">
+      <c r="B6" s="101" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:3">
-      <c r="A7" s="101" t="s">
+      <c r="A7" s="99" t="s">
         <v>105</v>
       </c>
-      <c r="B7" s="128" t="s">
+      <c r="B7" s="126" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="8" spans="1:3">
-      <c r="A8" s="103"/>
-      <c r="B8" s="71"/>
+      <c r="A8" s="101"/>
+      <c r="B8" s="69"/>
     </row>
     <row r="9" spans="1:3">
-      <c r="A9" s="103"/>
-      <c r="B9" s="71"/>
+      <c r="A9" s="101"/>
+      <c r="B9" s="69"/>
     </row>
     <row r="10" spans="1:3">
-      <c r="A10" s="67"/>
-      <c r="B10" s="67"/>
+      <c r="A10" s="65"/>
+      <c r="B10" s="65"/>
     </row>
     <row r="11" spans="1:3">
-      <c r="A11" s="72"/>
-      <c r="B11" s="71"/>
-      <c r="C11" s="88"/>
+      <c r="A11" s="70"/>
+      <c r="B11" s="69"/>
+      <c r="C11" s="86"/>
     </row>
     <row r="12" spans="1:3">
-      <c r="A12" s="67"/>
-      <c r="B12" s="103"/>
+      <c r="A12" s="65"/>
+      <c r="B12" s="101"/>
     </row>
     <row r="13" spans="1:3">
-      <c r="A13" s="104"/>
-      <c r="B13" s="103"/>
+      <c r="A13" s="102"/>
+      <c r="B13" s="101"/>
     </row>
     <row r="14" spans="1:3">
-      <c r="A14" s="118" t="s">
+      <c r="A14" s="116" t="s">
         <v>23</v>
       </c>
-      <c r="B14" s="104" t="s">
+      <c r="B14" s="102" t="s">
         <v>24</v>
       </c>
     </row>
@@ -5598,69 +5593,69 @@
       <c r="B17" t="s">
         <v>4</v>
       </c>
-      <c r="C17" s="125" t="s">
+      <c r="C17" s="123" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="18" spans="1:3" s="41" customFormat="1">
+    <row r="18" spans="1:3" s="39" customFormat="1">
       <c r="A18" s="10" t="s">
         <v>91</v>
       </c>
-      <c r="B18" s="41" t="s">
+      <c r="B18" s="39" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="19" spans="1:3" s="64" customFormat="1">
-      <c r="A19" s="94" t="s">
+    <row r="19" spans="1:3" s="62" customFormat="1">
+      <c r="A19" s="92" t="s">
         <v>100</v>
       </c>
-      <c r="B19" s="76" t="s">
+      <c r="B19" s="74" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="20" spans="1:3">
-      <c r="A20" s="118" t="s">
+      <c r="A20" s="116" t="s">
         <v>101</v>
       </c>
-      <c r="B20" s="101" t="s">
+      <c r="B20" s="99" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="21" spans="1:3">
-      <c r="A21" s="94" t="s">
+      <c r="A21" s="92" t="s">
         <v>101</v>
       </c>
-      <c r="B21" s="71" t="s">
+      <c r="B21" s="69" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="22" spans="1:3">
-      <c r="A22" s="118" t="s">
+      <c r="A22" s="116" t="s">
         <v>102</v>
       </c>
       <c r="B22" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="23" spans="1:3" s="49" customFormat="1">
-      <c r="A23" s="118" t="s">
+    <row r="23" spans="1:3" s="47" customFormat="1">
+      <c r="A23" s="116" t="s">
         <v>102</v>
       </c>
-      <c r="B23" s="49" t="s">
+      <c r="B23" s="47" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="24" spans="1:3">
-      <c r="A24" s="103"/>
+      <c r="A24" s="101"/>
       <c r="B24" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="25" spans="1:3">
-      <c r="A25" s="103" t="s">
+      <c r="A25" s="101" t="s">
         <v>13</v>
       </c>
-      <c r="B25" s="82" t="s">
+      <c r="B25" s="80" t="s">
         <v>14</v>
       </c>
     </row>
@@ -5668,60 +5663,60 @@
       <c r="A26" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="B26" s="100" t="s">
+      <c r="B26" s="98" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="27" spans="1:3">
-      <c r="A27" s="118" t="s">
+      <c r="A27" s="116" t="s">
         <v>92</v>
       </c>
-      <c r="B27" s="118" t="s">
+      <c r="B27" s="116" t="s">
         <v>99</v>
       </c>
     </row>
     <row r="28" spans="1:3">
-      <c r="A28" s="103" t="s">
+      <c r="A28" s="101" t="s">
         <v>16</v>
       </c>
-      <c r="B28" s="101" t="s">
+      <c r="B28" s="99" t="s">
         <v>17</v>
       </c>
-      <c r="C28" s="118" t="s">
+      <c r="C28" s="116" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="31" spans="1:3">
-      <c r="A31" s="118"/>
-      <c r="B31" s="118"/>
+      <c r="A31" s="116"/>
+      <c r="B31" s="116"/>
     </row>
     <row r="33" spans="1:3">
       <c r="A33" s="10" t="s">
         <v>93</v>
       </c>
-      <c r="B33" s="104" t="s">
+      <c r="B33" s="102" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="34" spans="1:3">
-      <c r="A34" s="94" t="s">
+      <c r="A34" s="92" t="s">
         <v>94</v>
       </c>
-      <c r="B34" s="71" t="s">
+      <c r="B34" s="69" t="s">
         <v>11</v>
       </c>
-      <c r="C34" s="118" t="s">
+      <c r="C34" s="116" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="35" spans="1:3">
-      <c r="A35" s="94" t="s">
+      <c r="A35" s="92" t="s">
         <v>94</v>
       </c>
-      <c r="B35" s="102" t="s">
+      <c r="B35" s="100" t="s">
         <v>11</v>
       </c>
-      <c r="C35" s="118" t="s">
+      <c r="C35" s="116" t="s">
         <v>90</v>
       </c>
     </row>
@@ -5758,41 +5753,41 @@
     <col min="7" max="7" width="10.875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="15.875" customWidth="1"/>
     <col min="9" max="9" width="17.375" customWidth="1"/>
-    <col min="10" max="10" width="9.875" style="50" customWidth="1"/>
-    <col min="11" max="11" width="9.875" style="48" customWidth="1"/>
+    <col min="10" max="10" width="9.875" style="48" customWidth="1"/>
+    <col min="11" max="11" width="9.875" style="46" customWidth="1"/>
     <col min="12" max="12" width="13.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="45" customFormat="1">
-      <c r="A1" s="45" t="s">
+    <row r="1" spans="1:12" s="43" customFormat="1">
+      <c r="A1" s="43" t="s">
         <v>70</v>
       </c>
-      <c r="J1" s="50"/>
-      <c r="K1" s="48"/>
-    </row>
-    <row r="2" spans="1:12" s="45" customFormat="1">
-      <c r="E2" s="149" t="s">
+      <c r="J1" s="48"/>
+      <c r="K1" s="46"/>
+    </row>
+    <row r="2" spans="1:12" s="43" customFormat="1">
+      <c r="E2" s="146" t="s">
         <v>71</v>
       </c>
-      <c r="F2" s="149"/>
-      <c r="G2" s="149"/>
-      <c r="H2" s="46" t="s">
+      <c r="F2" s="146"/>
+      <c r="G2" s="146"/>
+      <c r="H2" s="44" t="s">
         <v>72</v>
       </c>
-      <c r="I2" s="47">
+      <c r="I2" s="45">
         <v>0.45</v>
       </c>
-      <c r="J2" s="53"/>
-      <c r="K2" s="48"/>
+      <c r="J2" s="51"/>
+      <c r="K2" s="46"/>
     </row>
     <row r="3" spans="1:12" ht="24">
       <c r="B3" s="10" t="s">
         <v>73</v>
       </c>
-      <c r="C3" s="45" t="s">
+      <c r="C3" s="43" t="s">
         <v>74</v>
       </c>
-      <c r="D3" s="45" t="s">
+      <c r="D3" s="43" t="s">
         <v>75</v>
       </c>
       <c r="E3" s="10" t="s">
@@ -5807,72 +5802,72 @@
       <c r="H3" s="10" t="s">
         <v>115</v>
       </c>
-      <c r="I3" s="51" t="s">
+      <c r="I3" s="49" t="s">
         <v>78</v>
       </c>
-      <c r="J3" s="52" t="s">
+      <c r="J3" s="50" t="s">
         <v>79</v>
       </c>
-      <c r="K3" s="48" t="s">
+      <c r="K3" s="46" t="s">
         <v>80</v>
       </c>
       <c r="L3" s="10" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:12" s="56" customFormat="1">
+    <row r="4" spans="1:12" s="54" customFormat="1">
       <c r="A4" s="10" t="s">
         <v>81</v>
       </c>
       <c r="B4" s="10"/>
-      <c r="C4" s="129">
+      <c r="C4" s="127">
         <f>SMALL(C7:C100,COUNTIF($C$7:$C$100,0)+1)</f>
         <v>81000</v>
       </c>
-      <c r="D4" s="57">
+      <c r="D4" s="55">
         <f>MAX(D7:D121)</f>
         <v>83964</v>
       </c>
-      <c r="E4" s="130">
+      <c r="E4" s="128">
         <f>AVERAGEIF(E7:E1000,"&lt;&gt;0")</f>
         <v>76</v>
       </c>
-      <c r="F4" s="130">
+      <c r="F4" s="128">
         <f>AVERAGEIF(F7:F1000,"&lt;&gt;0")</f>
         <v>329.33333333333331</v>
       </c>
-      <c r="G4" s="87">
+      <c r="G4" s="85">
         <f>SUM(E7:E2073)</f>
         <v>2964</v>
       </c>
-      <c r="H4" s="130">
+      <c r="H4" s="128">
         <f>AVERAGEIF(H7:H1000,"&lt;&gt;0")</f>
         <v>148.19999999999999</v>
       </c>
-      <c r="I4" s="58">
+      <c r="I4" s="56">
         <f>MAX(I7:I329)</f>
         <v>1333.8</v>
       </c>
-      <c r="J4" s="58">
+      <c r="J4" s="56">
         <f>SUM(J7:J229)</f>
         <v>0</v>
       </c>
       <c r="L4" s="10"/>
     </row>
-    <row r="5" spans="1:12" s="68" customFormat="1">
+    <row r="5" spans="1:12" s="66" customFormat="1">
       <c r="A5" s="10"/>
       <c r="B5" s="10"/>
-      <c r="C5" s="57"/>
-      <c r="D5" s="57"/>
-      <c r="E5" s="57"/>
+      <c r="C5" s="55"/>
+      <c r="D5" s="55"/>
+      <c r="E5" s="55"/>
       <c r="F5" s="10"/>
       <c r="G5" s="10"/>
       <c r="H5" s="10"/>
-      <c r="I5" s="58"/>
-      <c r="J5" s="58"/>
+      <c r="I5" s="56"/>
+      <c r="J5" s="56"/>
       <c r="L5" s="10"/>
     </row>
-    <row r="6" spans="1:12" s="56" customFormat="1">
+    <row r="6" spans="1:12" s="54" customFormat="1">
       <c r="A6" s="10" t="s">
         <v>82</v>
       </c>
@@ -5881,1398 +5876,1398 @@
       <c r="F6" s="10"/>
       <c r="G6" s="10"/>
       <c r="H6" s="10"/>
-      <c r="I6" s="51"/>
-      <c r="J6" s="52"/>
+      <c r="I6" s="49"/>
+      <c r="J6" s="50"/>
       <c r="L6" s="10"/>
     </row>
     <row r="7" spans="1:12">
-      <c r="A7" s="142">
+      <c r="A7" s="139">
         <v>43692</v>
       </c>
-      <c r="B7" s="94" t="s">
+      <c r="B7" s="92" t="s">
         <v>83</v>
       </c>
-      <c r="C7" s="93"/>
-      <c r="D7" s="93"/>
-      <c r="E7" s="93">
+      <c r="C7" s="91"/>
+      <c r="D7" s="91"/>
+      <c r="E7" s="91">
         <v>0</v>
       </c>
-      <c r="F7" s="143">
+      <c r="F7" s="140">
         <f>SUM(E7:E11)</f>
         <v>228</v>
       </c>
-      <c r="G7" s="143">
+      <c r="G7" s="140">
         <f>F7</f>
         <v>228</v>
       </c>
-      <c r="H7" s="144">
+      <c r="H7" s="141">
         <f>F7*$I$2</f>
         <v>102.60000000000001</v>
       </c>
-      <c r="I7" s="144">
+      <c r="I7" s="141">
         <f>H7</f>
         <v>102.60000000000001</v>
       </c>
-      <c r="J7" s="95"/>
-      <c r="K7" s="95"/>
+      <c r="J7" s="93"/>
+      <c r="K7" s="93"/>
       <c r="L7" s="10"/>
     </row>
     <row r="8" spans="1:12">
-      <c r="A8" s="142"/>
-      <c r="B8" s="94" t="s">
+      <c r="A8" s="139"/>
+      <c r="B8" s="92" t="s">
         <v>84</v>
       </c>
-      <c r="C8" s="93"/>
-      <c r="D8" s="93"/>
-      <c r="E8" s="93">
+      <c r="C8" s="91"/>
+      <c r="D8" s="91"/>
+      <c r="E8" s="91">
         <v>0</v>
       </c>
-      <c r="F8" s="143"/>
-      <c r="G8" s="143"/>
-      <c r="H8" s="144"/>
-      <c r="I8" s="144"/>
-      <c r="J8" s="95"/>
-      <c r="K8" s="95"/>
-      <c r="L8" s="74"/>
+      <c r="F8" s="140"/>
+      <c r="G8" s="140"/>
+      <c r="H8" s="141"/>
+      <c r="I8" s="141"/>
+      <c r="J8" s="93"/>
+      <c r="K8" s="93"/>
+      <c r="L8" s="72"/>
     </row>
     <row r="9" spans="1:12">
-      <c r="A9" s="142"/>
-      <c r="B9" s="94" t="s">
+      <c r="A9" s="139"/>
+      <c r="B9" s="92" t="s">
         <v>85</v>
       </c>
-      <c r="C9" s="93">
+      <c r="C9" s="91">
         <v>81000</v>
       </c>
-      <c r="D9" s="93">
+      <c r="D9" s="91">
         <f>C9+E9</f>
         <v>81076</v>
       </c>
-      <c r="E9" s="93">
+      <c r="E9" s="91">
         <v>76</v>
       </c>
-      <c r="F9" s="143"/>
-      <c r="G9" s="143"/>
-      <c r="H9" s="144"/>
-      <c r="I9" s="144"/>
-      <c r="J9" s="95"/>
-      <c r="K9" s="95"/>
-      <c r="L9" s="74"/>
+      <c r="F9" s="140"/>
+      <c r="G9" s="140"/>
+      <c r="H9" s="141"/>
+      <c r="I9" s="141"/>
+      <c r="J9" s="93"/>
+      <c r="K9" s="93"/>
+      <c r="L9" s="72"/>
     </row>
     <row r="10" spans="1:12">
-      <c r="A10" s="142"/>
-      <c r="B10" s="94" t="s">
+      <c r="A10" s="139"/>
+      <c r="B10" s="92" t="s">
         <v>86</v>
       </c>
-      <c r="C10" s="93">
+      <c r="C10" s="91">
         <f>D9</f>
         <v>81076</v>
       </c>
-      <c r="D10" s="93">
+      <c r="D10" s="91">
         <f t="shared" ref="D10:D31" si="0">C10+E10</f>
         <v>81152</v>
       </c>
-      <c r="E10" s="93">
+      <c r="E10" s="91">
         <v>76</v>
       </c>
-      <c r="F10" s="143"/>
-      <c r="G10" s="143"/>
-      <c r="H10" s="144"/>
-      <c r="I10" s="144"/>
-      <c r="J10" s="95"/>
-      <c r="K10" s="95"/>
-      <c r="L10" s="74"/>
+      <c r="F10" s="140"/>
+      <c r="G10" s="140"/>
+      <c r="H10" s="141"/>
+      <c r="I10" s="141"/>
+      <c r="J10" s="93"/>
+      <c r="K10" s="93"/>
+      <c r="L10" s="72"/>
     </row>
     <row r="11" spans="1:12">
-      <c r="A11" s="142"/>
-      <c r="B11" s="94" t="s">
+      <c r="A11" s="139"/>
+      <c r="B11" s="92" t="s">
         <v>87</v>
       </c>
-      <c r="C11" s="93">
+      <c r="C11" s="91">
         <f t="shared" ref="C11:C31" si="1">D10</f>
         <v>81152</v>
       </c>
-      <c r="D11" s="93">
+      <c r="D11" s="91">
         <f t="shared" si="0"/>
         <v>81228</v>
       </c>
-      <c r="E11" s="93">
+      <c r="E11" s="91">
         <v>76</v>
       </c>
-      <c r="F11" s="143"/>
-      <c r="G11" s="143"/>
-      <c r="H11" s="144"/>
-      <c r="I11" s="144"/>
-      <c r="J11" s="95"/>
-      <c r="K11" s="95"/>
-      <c r="L11" s="74"/>
+      <c r="F11" s="140"/>
+      <c r="G11" s="140"/>
+      <c r="H11" s="141"/>
+      <c r="I11" s="141"/>
+      <c r="J11" s="93"/>
+      <c r="K11" s="93"/>
+      <c r="L11" s="72"/>
     </row>
     <row r="12" spans="1:12" ht="10.5" customHeight="1">
-      <c r="A12" s="145">
+      <c r="A12" s="142">
         <f>A7+7</f>
         <v>43699</v>
       </c>
-      <c r="B12" s="96" t="s">
+      <c r="B12" s="94" t="s">
         <v>83</v>
       </c>
-      <c r="C12" s="97">
+      <c r="C12" s="95">
         <f t="shared" si="1"/>
         <v>81228</v>
       </c>
-      <c r="D12" s="97">
+      <c r="D12" s="95">
         <f t="shared" si="0"/>
         <v>81304</v>
       </c>
-      <c r="E12" s="97">
+      <c r="E12" s="95">
         <v>76</v>
       </c>
-      <c r="F12" s="146">
+      <c r="F12" s="143">
         <f>SUM(E12:E16)</f>
         <v>380</v>
       </c>
-      <c r="G12" s="146">
+      <c r="G12" s="143">
         <f>G7+F12</f>
         <v>608</v>
       </c>
-      <c r="H12" s="147">
+      <c r="H12" s="144">
         <f>F12*$I$2</f>
         <v>171</v>
       </c>
-      <c r="I12" s="147">
+      <c r="I12" s="144">
         <f>I7+H12</f>
         <v>273.60000000000002</v>
       </c>
-      <c r="J12" s="98"/>
-      <c r="K12" s="98"/>
-      <c r="L12" s="74"/>
+      <c r="J12" s="96"/>
+      <c r="K12" s="96"/>
+      <c r="L12" s="72"/>
     </row>
     <row r="13" spans="1:12">
-      <c r="A13" s="145"/>
-      <c r="B13" s="96" t="s">
+      <c r="A13" s="142"/>
+      <c r="B13" s="94" t="s">
         <v>84</v>
       </c>
-      <c r="C13" s="97">
+      <c r="C13" s="95">
         <f t="shared" si="1"/>
         <v>81304</v>
       </c>
-      <c r="D13" s="97">
+      <c r="D13" s="95">
         <f t="shared" si="0"/>
         <v>81380</v>
       </c>
-      <c r="E13" s="97">
+      <c r="E13" s="95">
         <v>76</v>
       </c>
-      <c r="F13" s="146"/>
-      <c r="G13" s="146"/>
-      <c r="H13" s="147"/>
-      <c r="I13" s="147"/>
-      <c r="J13" s="98"/>
-      <c r="K13" s="98"/>
-      <c r="L13" s="74"/>
+      <c r="F13" s="143"/>
+      <c r="G13" s="143"/>
+      <c r="H13" s="144"/>
+      <c r="I13" s="144"/>
+      <c r="J13" s="96"/>
+      <c r="K13" s="96"/>
+      <c r="L13" s="72"/>
     </row>
     <row r="14" spans="1:12">
-      <c r="A14" s="145"/>
-      <c r="B14" s="96" t="s">
+      <c r="A14" s="142"/>
+      <c r="B14" s="94" t="s">
         <v>85</v>
       </c>
-      <c r="C14" s="97">
+      <c r="C14" s="95">
         <f t="shared" si="1"/>
         <v>81380</v>
       </c>
-      <c r="D14" s="97">
+      <c r="D14" s="95">
         <f t="shared" si="0"/>
         <v>81456</v>
       </c>
-      <c r="E14" s="97">
+      <c r="E14" s="95">
         <v>76</v>
       </c>
-      <c r="F14" s="146"/>
-      <c r="G14" s="146"/>
-      <c r="H14" s="147"/>
-      <c r="I14" s="147"/>
-      <c r="J14" s="98"/>
-      <c r="K14" s="98"/>
-      <c r="L14" s="74"/>
+      <c r="F14" s="143"/>
+      <c r="G14" s="143"/>
+      <c r="H14" s="144"/>
+      <c r="I14" s="144"/>
+      <c r="J14" s="96"/>
+      <c r="K14" s="96"/>
+      <c r="L14" s="72"/>
     </row>
     <row r="15" spans="1:12">
-      <c r="A15" s="145"/>
-      <c r="B15" s="96" t="s">
+      <c r="A15" s="142"/>
+      <c r="B15" s="94" t="s">
         <v>86</v>
       </c>
-      <c r="C15" s="97">
+      <c r="C15" s="95">
         <f t="shared" si="1"/>
         <v>81456</v>
       </c>
-      <c r="D15" s="97">
+      <c r="D15" s="95">
         <f t="shared" si="0"/>
         <v>81532</v>
       </c>
-      <c r="E15" s="97">
+      <c r="E15" s="95">
         <v>76</v>
       </c>
-      <c r="F15" s="146"/>
-      <c r="G15" s="146"/>
-      <c r="H15" s="147"/>
-      <c r="I15" s="147"/>
-      <c r="J15" s="98"/>
-      <c r="K15" s="98"/>
-      <c r="L15" s="74"/>
+      <c r="F15" s="143"/>
+      <c r="G15" s="143"/>
+      <c r="H15" s="144"/>
+      <c r="I15" s="144"/>
+      <c r="J15" s="96"/>
+      <c r="K15" s="96"/>
+      <c r="L15" s="72"/>
     </row>
     <row r="16" spans="1:12">
-      <c r="A16" s="145"/>
-      <c r="B16" s="96" t="s">
+      <c r="A16" s="142"/>
+      <c r="B16" s="94" t="s">
         <v>87</v>
       </c>
-      <c r="C16" s="97">
+      <c r="C16" s="95">
         <f t="shared" si="1"/>
         <v>81532</v>
       </c>
-      <c r="D16" s="97">
+      <c r="D16" s="95">
         <f t="shared" si="0"/>
         <v>81608</v>
       </c>
-      <c r="E16" s="97">
+      <c r="E16" s="95">
         <v>76</v>
       </c>
-      <c r="F16" s="146"/>
-      <c r="G16" s="146"/>
-      <c r="H16" s="147"/>
-      <c r="I16" s="147"/>
-      <c r="J16" s="98"/>
-      <c r="K16" s="98"/>
+      <c r="F16" s="143"/>
+      <c r="G16" s="143"/>
+      <c r="H16" s="144"/>
+      <c r="I16" s="144"/>
+      <c r="J16" s="96"/>
+      <c r="K16" s="96"/>
       <c r="L16" s="10"/>
     </row>
     <row r="17" spans="1:12">
-      <c r="A17" s="142">
+      <c r="A17" s="139">
         <f>A12+7</f>
         <v>43706</v>
       </c>
-      <c r="B17" s="94" t="s">
+      <c r="B17" s="92" t="s">
         <v>83</v>
       </c>
-      <c r="C17" s="93"/>
-      <c r="D17" s="93"/>
-      <c r="E17" s="93"/>
-      <c r="F17" s="143">
+      <c r="C17" s="91"/>
+      <c r="D17" s="91"/>
+      <c r="E17" s="91"/>
+      <c r="F17" s="140">
         <f>SUM(E17:E21)</f>
         <v>304</v>
       </c>
-      <c r="G17" s="143">
+      <c r="G17" s="140">
         <f>G12+F17</f>
         <v>912</v>
       </c>
-      <c r="H17" s="144">
+      <c r="H17" s="141">
         <f>F17*$I$2</f>
         <v>136.80000000000001</v>
       </c>
-      <c r="I17" s="144">
+      <c r="I17" s="141">
         <f>I12+H17</f>
         <v>410.40000000000003</v>
       </c>
-      <c r="J17" s="95"/>
-      <c r="K17" s="95"/>
-      <c r="L17" s="74"/>
+      <c r="J17" s="93"/>
+      <c r="K17" s="93"/>
+      <c r="L17" s="72"/>
     </row>
     <row r="18" spans="1:12">
-      <c r="A18" s="142"/>
-      <c r="B18" s="94" t="s">
+      <c r="A18" s="139"/>
+      <c r="B18" s="92" t="s">
         <v>84</v>
       </c>
-      <c r="C18" s="93">
+      <c r="C18" s="91">
         <f>D16</f>
         <v>81608</v>
       </c>
-      <c r="D18" s="93">
+      <c r="D18" s="91">
         <f t="shared" si="0"/>
         <v>81684</v>
       </c>
-      <c r="E18" s="93">
+      <c r="E18" s="91">
         <v>76</v>
       </c>
-      <c r="F18" s="143"/>
-      <c r="G18" s="143"/>
-      <c r="H18" s="144"/>
-      <c r="I18" s="144"/>
-      <c r="J18" s="95"/>
-      <c r="K18" s="95"/>
-      <c r="L18" s="74"/>
+      <c r="F18" s="140"/>
+      <c r="G18" s="140"/>
+      <c r="H18" s="141"/>
+      <c r="I18" s="141"/>
+      <c r="J18" s="93"/>
+      <c r="K18" s="93"/>
+      <c r="L18" s="72"/>
     </row>
     <row r="19" spans="1:12">
-      <c r="A19" s="142"/>
-      <c r="B19" s="94" t="s">
+      <c r="A19" s="139"/>
+      <c r="B19" s="92" t="s">
         <v>85</v>
       </c>
-      <c r="C19" s="93">
+      <c r="C19" s="91">
         <f t="shared" si="1"/>
         <v>81684</v>
       </c>
-      <c r="D19" s="93">
+      <c r="D19" s="91">
         <f t="shared" si="0"/>
         <v>81760</v>
       </c>
-      <c r="E19" s="93">
+      <c r="E19" s="91">
         <v>76</v>
       </c>
-      <c r="F19" s="143"/>
-      <c r="G19" s="143"/>
-      <c r="H19" s="144"/>
-      <c r="I19" s="144"/>
-      <c r="J19" s="95"/>
-      <c r="K19" s="95"/>
-      <c r="L19" s="74"/>
+      <c r="F19" s="140"/>
+      <c r="G19" s="140"/>
+      <c r="H19" s="141"/>
+      <c r="I19" s="141"/>
+      <c r="J19" s="93"/>
+      <c r="K19" s="93"/>
+      <c r="L19" s="72"/>
     </row>
     <row r="20" spans="1:12">
-      <c r="A20" s="142"/>
-      <c r="B20" s="94" t="s">
+      <c r="A20" s="139"/>
+      <c r="B20" s="92" t="s">
         <v>86</v>
       </c>
-      <c r="C20" s="93">
+      <c r="C20" s="91">
         <f t="shared" si="1"/>
         <v>81760</v>
       </c>
-      <c r="D20" s="93">
+      <c r="D20" s="91">
         <f t="shared" si="0"/>
         <v>81836</v>
       </c>
-      <c r="E20" s="93">
+      <c r="E20" s="91">
         <v>76</v>
       </c>
-      <c r="F20" s="143"/>
-      <c r="G20" s="143"/>
-      <c r="H20" s="144"/>
-      <c r="I20" s="144"/>
-      <c r="J20" s="95"/>
-      <c r="K20" s="95"/>
-      <c r="L20" s="74"/>
+      <c r="F20" s="140"/>
+      <c r="G20" s="140"/>
+      <c r="H20" s="141"/>
+      <c r="I20" s="141"/>
+      <c r="J20" s="93"/>
+      <c r="K20" s="93"/>
+      <c r="L20" s="72"/>
     </row>
     <row r="21" spans="1:12">
-      <c r="A21" s="142"/>
-      <c r="B21" s="94" t="s">
+      <c r="A21" s="139"/>
+      <c r="B21" s="92" t="s">
         <v>87</v>
       </c>
-      <c r="C21" s="93">
+      <c r="C21" s="91">
         <f t="shared" si="1"/>
         <v>81836</v>
       </c>
-      <c r="D21" s="93">
+      <c r="D21" s="91">
         <f t="shared" si="0"/>
         <v>81912</v>
       </c>
-      <c r="E21" s="93">
+      <c r="E21" s="91">
         <v>76</v>
       </c>
-      <c r="F21" s="143"/>
-      <c r="G21" s="143"/>
-      <c r="H21" s="144"/>
-      <c r="I21" s="144"/>
-      <c r="J21" s="95"/>
-      <c r="K21" s="95"/>
-      <c r="L21" s="74"/>
+      <c r="F21" s="140"/>
+      <c r="G21" s="140"/>
+      <c r="H21" s="141"/>
+      <c r="I21" s="141"/>
+      <c r="J21" s="93"/>
+      <c r="K21" s="93"/>
+      <c r="L21" s="72"/>
     </row>
     <row r="22" spans="1:12">
-      <c r="A22" s="145">
+      <c r="A22" s="142">
         <f>A17+7</f>
         <v>43713</v>
       </c>
-      <c r="B22" s="96" t="s">
+      <c r="B22" s="94" t="s">
         <v>83</v>
       </c>
-      <c r="C22" s="97">
+      <c r="C22" s="95">
         <f t="shared" si="1"/>
         <v>81912</v>
       </c>
-      <c r="D22" s="97">
+      <c r="D22" s="95">
         <f t="shared" si="0"/>
         <v>81988</v>
       </c>
-      <c r="E22" s="97">
+      <c r="E22" s="95">
         <v>76</v>
       </c>
-      <c r="F22" s="146">
+      <c r="F22" s="143">
         <f>SUM(E22:E26)</f>
         <v>380</v>
       </c>
-      <c r="G22" s="146">
+      <c r="G22" s="143">
         <f>G17+F22</f>
         <v>1292</v>
       </c>
-      <c r="H22" s="147">
+      <c r="H22" s="144">
         <f>F22*$I$2</f>
         <v>171</v>
       </c>
-      <c r="I22" s="147">
+      <c r="I22" s="144">
         <f>I17+H22</f>
         <v>581.40000000000009</v>
       </c>
-      <c r="J22" s="98"/>
-      <c r="K22" s="98"/>
+      <c r="J22" s="96"/>
+      <c r="K22" s="96"/>
       <c r="L22" s="10"/>
     </row>
     <row r="23" spans="1:12">
-      <c r="A23" s="145"/>
-      <c r="B23" s="96" t="s">
+      <c r="A23" s="142"/>
+      <c r="B23" s="94" t="s">
         <v>84</v>
       </c>
-      <c r="C23" s="97">
+      <c r="C23" s="95">
         <f t="shared" si="1"/>
         <v>81988</v>
       </c>
-      <c r="D23" s="97">
+      <c r="D23" s="95">
         <f t="shared" si="0"/>
         <v>82064</v>
       </c>
-      <c r="E23" s="97">
+      <c r="E23" s="95">
         <v>76</v>
       </c>
-      <c r="F23" s="146"/>
-      <c r="G23" s="146"/>
-      <c r="H23" s="147"/>
-      <c r="I23" s="147"/>
-      <c r="J23" s="98"/>
-      <c r="K23" s="98"/>
-      <c r="L23" s="74"/>
+      <c r="F23" s="143"/>
+      <c r="G23" s="143"/>
+      <c r="H23" s="144"/>
+      <c r="I23" s="144"/>
+      <c r="J23" s="96"/>
+      <c r="K23" s="96"/>
+      <c r="L23" s="72"/>
     </row>
     <row r="24" spans="1:12">
-      <c r="A24" s="145"/>
-      <c r="B24" s="96" t="s">
+      <c r="A24" s="142"/>
+      <c r="B24" s="94" t="s">
         <v>85</v>
       </c>
-      <c r="C24" s="97">
+      <c r="C24" s="95">
         <f t="shared" si="1"/>
         <v>82064</v>
       </c>
-      <c r="D24" s="97">
+      <c r="D24" s="95">
         <f t="shared" si="0"/>
         <v>82140</v>
       </c>
-      <c r="E24" s="97">
+      <c r="E24" s="95">
         <v>76</v>
       </c>
-      <c r="F24" s="146"/>
-      <c r="G24" s="146"/>
-      <c r="H24" s="147"/>
-      <c r="I24" s="147"/>
-      <c r="J24" s="98"/>
-      <c r="K24" s="98"/>
-      <c r="L24" s="74"/>
+      <c r="F24" s="143"/>
+      <c r="G24" s="143"/>
+      <c r="H24" s="144"/>
+      <c r="I24" s="144"/>
+      <c r="J24" s="96"/>
+      <c r="K24" s="96"/>
+      <c r="L24" s="72"/>
     </row>
     <row r="25" spans="1:12">
-      <c r="A25" s="145"/>
-      <c r="B25" s="96" t="s">
+      <c r="A25" s="142"/>
+      <c r="B25" s="94" t="s">
         <v>86</v>
       </c>
-      <c r="C25" s="97">
+      <c r="C25" s="95">
         <f t="shared" si="1"/>
         <v>82140</v>
       </c>
-      <c r="D25" s="97">
+      <c r="D25" s="95">
         <f t="shared" si="0"/>
         <v>82216</v>
       </c>
-      <c r="E25" s="97">
+      <c r="E25" s="95">
         <v>76</v>
       </c>
-      <c r="F25" s="146"/>
-      <c r="G25" s="146"/>
-      <c r="H25" s="147"/>
-      <c r="I25" s="147"/>
-      <c r="J25" s="98"/>
-      <c r="K25" s="98"/>
-      <c r="L25" s="74"/>
+      <c r="F25" s="143"/>
+      <c r="G25" s="143"/>
+      <c r="H25" s="144"/>
+      <c r="I25" s="144"/>
+      <c r="J25" s="96"/>
+      <c r="K25" s="96"/>
+      <c r="L25" s="72"/>
     </row>
     <row r="26" spans="1:12">
-      <c r="A26" s="145"/>
-      <c r="B26" s="96" t="s">
+      <c r="A26" s="142"/>
+      <c r="B26" s="94" t="s">
         <v>87</v>
       </c>
-      <c r="C26" s="97">
+      <c r="C26" s="95">
         <f t="shared" si="1"/>
         <v>82216</v>
       </c>
-      <c r="D26" s="97">
+      <c r="D26" s="95">
         <f t="shared" si="0"/>
         <v>82292</v>
       </c>
-      <c r="E26" s="97">
+      <c r="E26" s="95">
         <v>76</v>
       </c>
-      <c r="F26" s="146"/>
-      <c r="G26" s="146"/>
-      <c r="H26" s="147"/>
-      <c r="I26" s="147"/>
-      <c r="J26" s="98"/>
-      <c r="K26" s="98"/>
-      <c r="L26" s="74"/>
+      <c r="F26" s="143"/>
+      <c r="G26" s="143"/>
+      <c r="H26" s="144"/>
+      <c r="I26" s="144"/>
+      <c r="J26" s="96"/>
+      <c r="K26" s="96"/>
+      <c r="L26" s="72"/>
     </row>
     <row r="27" spans="1:12">
-      <c r="A27" s="142">
+      <c r="A27" s="139">
         <f>A22+7</f>
         <v>43720</v>
       </c>
-      <c r="B27" s="94" t="s">
+      <c r="B27" s="92" t="s">
         <v>83</v>
       </c>
-      <c r="C27" s="93">
+      <c r="C27" s="91">
         <f t="shared" si="1"/>
         <v>82292</v>
       </c>
-      <c r="D27" s="93">
+      <c r="D27" s="91">
         <f t="shared" si="0"/>
         <v>82368</v>
       </c>
-      <c r="E27" s="93">
+      <c r="E27" s="91">
         <v>76</v>
       </c>
-      <c r="F27" s="143">
+      <c r="F27" s="140">
         <f>SUM(E27:E31)</f>
         <v>380</v>
       </c>
-      <c r="G27" s="143">
+      <c r="G27" s="140">
         <f>G22+F27</f>
         <v>1672</v>
       </c>
-      <c r="H27" s="144">
+      <c r="H27" s="141">
         <f>F27*$I$2</f>
         <v>171</v>
       </c>
-      <c r="I27" s="144">
+      <c r="I27" s="141">
         <f>I22+H27</f>
         <v>752.40000000000009</v>
       </c>
-      <c r="J27" s="95"/>
-      <c r="K27" s="95"/>
-      <c r="L27" s="74"/>
+      <c r="J27" s="93"/>
+      <c r="K27" s="93"/>
+      <c r="L27" s="72"/>
     </row>
     <row r="28" spans="1:12">
-      <c r="A28" s="142"/>
-      <c r="B28" s="94" t="s">
+      <c r="A28" s="139"/>
+      <c r="B28" s="92" t="s">
         <v>84</v>
       </c>
-      <c r="C28" s="93">
+      <c r="C28" s="91">
         <f t="shared" si="1"/>
         <v>82368</v>
       </c>
-      <c r="D28" s="93">
+      <c r="D28" s="91">
         <f t="shared" si="0"/>
         <v>82444</v>
       </c>
-      <c r="E28" s="93">
+      <c r="E28" s="91">
         <v>76</v>
       </c>
-      <c r="F28" s="143"/>
-      <c r="G28" s="143"/>
-      <c r="H28" s="144"/>
-      <c r="I28" s="144"/>
-      <c r="J28" s="95"/>
-      <c r="K28" s="95"/>
-      <c r="L28" s="74"/>
+      <c r="F28" s="140"/>
+      <c r="G28" s="140"/>
+      <c r="H28" s="141"/>
+      <c r="I28" s="141"/>
+      <c r="J28" s="93"/>
+      <c r="K28" s="93"/>
+      <c r="L28" s="72"/>
     </row>
     <row r="29" spans="1:12">
-      <c r="A29" s="142"/>
-      <c r="B29" s="94" t="s">
+      <c r="A29" s="139"/>
+      <c r="B29" s="92" t="s">
         <v>85</v>
       </c>
-      <c r="C29" s="93">
+      <c r="C29" s="91">
         <f t="shared" si="1"/>
         <v>82444</v>
       </c>
-      <c r="D29" s="93">
+      <c r="D29" s="91">
         <f t="shared" si="0"/>
         <v>82520</v>
       </c>
-      <c r="E29" s="93">
+      <c r="E29" s="91">
         <v>76</v>
       </c>
-      <c r="F29" s="143"/>
-      <c r="G29" s="143"/>
-      <c r="H29" s="144"/>
-      <c r="I29" s="144"/>
-      <c r="J29" s="95"/>
-      <c r="K29" s="95"/>
-      <c r="L29" s="74"/>
+      <c r="F29" s="140"/>
+      <c r="G29" s="140"/>
+      <c r="H29" s="141"/>
+      <c r="I29" s="141"/>
+      <c r="J29" s="93"/>
+      <c r="K29" s="93"/>
+      <c r="L29" s="72"/>
     </row>
     <row r="30" spans="1:12">
-      <c r="A30" s="142"/>
-      <c r="B30" s="94" t="s">
+      <c r="A30" s="139"/>
+      <c r="B30" s="92" t="s">
         <v>86</v>
       </c>
-      <c r="C30" s="93">
+      <c r="C30" s="91">
         <f t="shared" si="1"/>
         <v>82520</v>
       </c>
-      <c r="D30" s="93">
+      <c r="D30" s="91">
         <f t="shared" si="0"/>
         <v>82596</v>
       </c>
-      <c r="E30" s="93">
+      <c r="E30" s="91">
         <v>76</v>
       </c>
-      <c r="F30" s="143"/>
-      <c r="G30" s="143"/>
-      <c r="H30" s="144"/>
-      <c r="I30" s="144"/>
-      <c r="J30" s="95"/>
-      <c r="K30" s="95"/>
-      <c r="L30" s="74"/>
+      <c r="F30" s="140"/>
+      <c r="G30" s="140"/>
+      <c r="H30" s="141"/>
+      <c r="I30" s="141"/>
+      <c r="J30" s="93"/>
+      <c r="K30" s="93"/>
+      <c r="L30" s="72"/>
     </row>
     <row r="31" spans="1:12">
-      <c r="A31" s="142"/>
-      <c r="B31" s="94" t="s">
+      <c r="A31" s="139"/>
+      <c r="B31" s="92" t="s">
         <v>87</v>
       </c>
-      <c r="C31" s="93">
+      <c r="C31" s="91">
         <f t="shared" si="1"/>
         <v>82596</v>
       </c>
-      <c r="D31" s="93">
+      <c r="D31" s="91">
         <f t="shared" si="0"/>
         <v>82672</v>
       </c>
-      <c r="E31" s="93">
+      <c r="E31" s="91">
         <v>76</v>
       </c>
-      <c r="F31" s="143"/>
-      <c r="G31" s="143"/>
-      <c r="H31" s="144"/>
-      <c r="I31" s="144"/>
-      <c r="J31" s="95"/>
-      <c r="K31" s="95"/>
-      <c r="L31" s="74"/>
+      <c r="F31" s="140"/>
+      <c r="G31" s="140"/>
+      <c r="H31" s="141"/>
+      <c r="I31" s="141"/>
+      <c r="J31" s="93"/>
+      <c r="K31" s="93"/>
+      <c r="L31" s="72"/>
     </row>
     <row r="32" spans="1:12">
-      <c r="A32" s="145">
+      <c r="A32" s="142">
         <f>A27+7</f>
         <v>43727</v>
       </c>
-      <c r="B32" s="96" t="s">
+      <c r="B32" s="94" t="s">
         <v>83</v>
       </c>
-      <c r="C32" s="97"/>
-      <c r="D32" s="97"/>
-      <c r="E32" s="97">
+      <c r="C32" s="95"/>
+      <c r="D32" s="95"/>
+      <c r="E32" s="95">
         <v>0</v>
       </c>
-      <c r="F32" s="148">
+      <c r="F32" s="145">
         <f>SUM(E32:E36)</f>
         <v>304</v>
       </c>
-      <c r="G32" s="148">
+      <c r="G32" s="145">
         <f>G27+F32</f>
         <v>1976</v>
       </c>
-      <c r="H32" s="147">
+      <c r="H32" s="144">
         <f>F32*$I$2</f>
         <v>136.80000000000001</v>
       </c>
-      <c r="I32" s="147">
+      <c r="I32" s="144">
         <f>I27+H32</f>
         <v>889.2</v>
       </c>
-      <c r="J32" s="98"/>
-      <c r="K32" s="98"/>
-      <c r="L32" s="117"/>
+      <c r="J32" s="96"/>
+      <c r="K32" s="96"/>
+      <c r="L32" s="115"/>
     </row>
     <row r="33" spans="1:12">
-      <c r="A33" s="145"/>
-      <c r="B33" s="96" t="s">
+      <c r="A33" s="142"/>
+      <c r="B33" s="94" t="s">
         <v>84</v>
       </c>
-      <c r="C33" s="97">
+      <c r="C33" s="95">
         <f>D31</f>
         <v>82672</v>
       </c>
-      <c r="D33" s="97">
+      <c r="D33" s="95">
         <f t="shared" ref="D33:D50" si="2">C33+E33</f>
         <v>82748</v>
       </c>
-      <c r="E33" s="97">
+      <c r="E33" s="95">
         <v>76</v>
       </c>
-      <c r="F33" s="148"/>
-      <c r="G33" s="148"/>
-      <c r="H33" s="147"/>
-      <c r="I33" s="147"/>
-      <c r="J33" s="98"/>
-      <c r="K33" s="98"/>
+      <c r="F33" s="145"/>
+      <c r="G33" s="145"/>
+      <c r="H33" s="144"/>
+      <c r="I33" s="144"/>
+      <c r="J33" s="96"/>
+      <c r="K33" s="96"/>
     </row>
     <row r="34" spans="1:12">
-      <c r="A34" s="145"/>
-      <c r="B34" s="96" t="s">
+      <c r="A34" s="142"/>
+      <c r="B34" s="94" t="s">
         <v>85</v>
       </c>
-      <c r="C34" s="97">
+      <c r="C34" s="95">
         <f t="shared" ref="C34:C50" si="3">D33</f>
         <v>82748</v>
       </c>
-      <c r="D34" s="97">
+      <c r="D34" s="95">
         <f t="shared" si="2"/>
         <v>82824</v>
       </c>
-      <c r="E34" s="97">
+      <c r="E34" s="95">
         <v>76</v>
       </c>
-      <c r="F34" s="148"/>
-      <c r="G34" s="148"/>
-      <c r="H34" s="147"/>
-      <c r="I34" s="147"/>
-      <c r="J34" s="98"/>
-      <c r="K34" s="98"/>
+      <c r="F34" s="145"/>
+      <c r="G34" s="145"/>
+      <c r="H34" s="144"/>
+      <c r="I34" s="144"/>
+      <c r="J34" s="96"/>
+      <c r="K34" s="96"/>
     </row>
     <row r="35" spans="1:12">
-      <c r="A35" s="145"/>
-      <c r="B35" s="96" t="s">
+      <c r="A35" s="142"/>
+      <c r="B35" s="94" t="s">
         <v>86</v>
       </c>
-      <c r="C35" s="97">
+      <c r="C35" s="95">
         <f t="shared" si="3"/>
         <v>82824</v>
       </c>
-      <c r="D35" s="97">
+      <c r="D35" s="95">
         <f t="shared" si="2"/>
         <v>82900</v>
       </c>
-      <c r="E35" s="97">
+      <c r="E35" s="95">
         <v>76</v>
       </c>
-      <c r="F35" s="148"/>
-      <c r="G35" s="148"/>
-      <c r="H35" s="147"/>
-      <c r="I35" s="147"/>
-      <c r="J35" s="98"/>
-      <c r="K35" s="98"/>
+      <c r="F35" s="145"/>
+      <c r="G35" s="145"/>
+      <c r="H35" s="144"/>
+      <c r="I35" s="144"/>
+      <c r="J35" s="96"/>
+      <c r="K35" s="96"/>
     </row>
     <row r="36" spans="1:12">
-      <c r="A36" s="145"/>
-      <c r="B36" s="96" t="s">
+      <c r="A36" s="142"/>
+      <c r="B36" s="94" t="s">
         <v>87</v>
       </c>
-      <c r="C36" s="97">
+      <c r="C36" s="95">
         <f t="shared" si="3"/>
         <v>82900</v>
       </c>
-      <c r="D36" s="97">
+      <c r="D36" s="95">
         <f t="shared" si="2"/>
         <v>82976</v>
       </c>
-      <c r="E36" s="97">
+      <c r="E36" s="95">
         <v>76</v>
       </c>
-      <c r="F36" s="148"/>
-      <c r="G36" s="148"/>
-      <c r="H36" s="147"/>
-      <c r="I36" s="147"/>
-      <c r="J36" s="98"/>
-      <c r="K36" s="98"/>
+      <c r="F36" s="145"/>
+      <c r="G36" s="145"/>
+      <c r="H36" s="144"/>
+      <c r="I36" s="144"/>
+      <c r="J36" s="96"/>
+      <c r="K36" s="96"/>
     </row>
     <row r="37" spans="1:12">
-      <c r="A37" s="142">
+      <c r="A37" s="139">
         <f>A32+7</f>
         <v>43734</v>
       </c>
-      <c r="B37" s="94" t="s">
+      <c r="B37" s="92" t="s">
         <v>83</v>
       </c>
-      <c r="C37" s="93">
+      <c r="C37" s="91">
         <f t="shared" si="3"/>
         <v>82976</v>
       </c>
-      <c r="D37" s="93">
+      <c r="D37" s="91">
         <f t="shared" si="2"/>
         <v>83052</v>
       </c>
-      <c r="E37" s="93">
+      <c r="E37" s="91">
         <v>76</v>
       </c>
-      <c r="F37" s="143">
+      <c r="F37" s="140">
         <f>SUM(E37:E41)</f>
         <v>380</v>
       </c>
-      <c r="G37" s="143">
+      <c r="G37" s="140">
         <f>G32+F37</f>
         <v>2356</v>
       </c>
-      <c r="H37" s="144">
+      <c r="H37" s="141">
         <f>F37*$I$2</f>
         <v>171</v>
       </c>
-      <c r="I37" s="144">
+      <c r="I37" s="141">
         <f>I32+H37</f>
         <v>1060.2</v>
       </c>
-      <c r="J37" s="95"/>
-      <c r="K37" s="95"/>
+      <c r="J37" s="93"/>
+      <c r="K37" s="93"/>
     </row>
     <row r="38" spans="1:12">
-      <c r="A38" s="142"/>
-      <c r="B38" s="94" t="s">
+      <c r="A38" s="139"/>
+      <c r="B38" s="92" t="s">
         <v>84</v>
       </c>
-      <c r="C38" s="93">
+      <c r="C38" s="91">
         <f t="shared" si="3"/>
         <v>83052</v>
       </c>
-      <c r="D38" s="93">
+      <c r="D38" s="91">
         <f t="shared" si="2"/>
         <v>83128</v>
       </c>
-      <c r="E38" s="93">
+      <c r="E38" s="91">
         <v>76</v>
       </c>
-      <c r="F38" s="143"/>
-      <c r="G38" s="143"/>
-      <c r="H38" s="144"/>
-      <c r="I38" s="144"/>
-      <c r="J38" s="95"/>
-      <c r="K38" s="95"/>
+      <c r="F38" s="140"/>
+      <c r="G38" s="140"/>
+      <c r="H38" s="141"/>
+      <c r="I38" s="141"/>
+      <c r="J38" s="93"/>
+      <c r="K38" s="93"/>
     </row>
     <row r="39" spans="1:12">
-      <c r="A39" s="142"/>
-      <c r="B39" s="94" t="s">
+      <c r="A39" s="139"/>
+      <c r="B39" s="92" t="s">
         <v>85</v>
       </c>
-      <c r="C39" s="93">
+      <c r="C39" s="91">
         <f t="shared" si="3"/>
         <v>83128</v>
       </c>
-      <c r="D39" s="93">
+      <c r="D39" s="91">
         <f t="shared" si="2"/>
         <v>83204</v>
       </c>
-      <c r="E39" s="93">
+      <c r="E39" s="91">
         <v>76</v>
       </c>
-      <c r="F39" s="143"/>
-      <c r="G39" s="143"/>
-      <c r="H39" s="144"/>
-      <c r="I39" s="144"/>
-      <c r="J39" s="95"/>
-      <c r="K39" s="95"/>
+      <c r="F39" s="140"/>
+      <c r="G39" s="140"/>
+      <c r="H39" s="141"/>
+      <c r="I39" s="141"/>
+      <c r="J39" s="93"/>
+      <c r="K39" s="93"/>
     </row>
     <row r="40" spans="1:12">
-      <c r="A40" s="142"/>
-      <c r="B40" s="94" t="s">
+      <c r="A40" s="139"/>
+      <c r="B40" s="92" t="s">
         <v>86</v>
       </c>
-      <c r="C40" s="93">
+      <c r="C40" s="91">
         <f t="shared" si="3"/>
         <v>83204</v>
       </c>
-      <c r="D40" s="93">
+      <c r="D40" s="91">
         <f t="shared" si="2"/>
         <v>83280</v>
       </c>
-      <c r="E40" s="93">
+      <c r="E40" s="91">
         <v>76</v>
       </c>
-      <c r="F40" s="143"/>
-      <c r="G40" s="143"/>
-      <c r="H40" s="144"/>
-      <c r="I40" s="144"/>
-      <c r="J40" s="95"/>
-      <c r="K40" s="95"/>
+      <c r="F40" s="140"/>
+      <c r="G40" s="140"/>
+      <c r="H40" s="141"/>
+      <c r="I40" s="141"/>
+      <c r="J40" s="93"/>
+      <c r="K40" s="93"/>
     </row>
     <row r="41" spans="1:12">
-      <c r="A41" s="142"/>
-      <c r="B41" s="94" t="s">
+      <c r="A41" s="139"/>
+      <c r="B41" s="92" t="s">
         <v>87</v>
       </c>
-      <c r="C41" s="93">
+      <c r="C41" s="91">
         <f t="shared" si="3"/>
         <v>83280</v>
       </c>
-      <c r="D41" s="93">
+      <c r="D41" s="91">
         <f t="shared" si="2"/>
         <v>83356</v>
       </c>
-      <c r="E41" s="93">
+      <c r="E41" s="91">
         <v>76</v>
       </c>
-      <c r="F41" s="143"/>
-      <c r="G41" s="143"/>
-      <c r="H41" s="144"/>
-      <c r="I41" s="144"/>
-      <c r="J41" s="95"/>
-      <c r="K41" s="95"/>
+      <c r="F41" s="140"/>
+      <c r="G41" s="140"/>
+      <c r="H41" s="141"/>
+      <c r="I41" s="141"/>
+      <c r="J41" s="93"/>
+      <c r="K41" s="93"/>
     </row>
     <row r="42" spans="1:12">
-      <c r="A42" s="145">
+      <c r="A42" s="142">
         <f>A37+7</f>
         <v>43741</v>
       </c>
-      <c r="B42" s="96" t="s">
+      <c r="B42" s="94" t="s">
         <v>83</v>
       </c>
-      <c r="C42" s="97">
+      <c r="C42" s="95">
         <f t="shared" si="3"/>
         <v>83356</v>
       </c>
-      <c r="D42" s="97">
+      <c r="D42" s="95">
         <f t="shared" si="2"/>
         <v>83432</v>
       </c>
-      <c r="E42" s="97">
+      <c r="E42" s="95">
         <v>76</v>
       </c>
-      <c r="F42" s="148">
+      <c r="F42" s="145">
         <f>SUM(E42:E46)</f>
         <v>304</v>
       </c>
-      <c r="G42" s="148">
+      <c r="G42" s="145">
         <f>G37+F42</f>
         <v>2660</v>
       </c>
-      <c r="H42" s="147">
+      <c r="H42" s="144">
         <f>F42*$I$2</f>
         <v>136.80000000000001</v>
       </c>
-      <c r="I42" s="147">
+      <c r="I42" s="144">
         <f>I37+H42</f>
         <v>1197</v>
       </c>
-      <c r="J42" s="98"/>
-      <c r="K42" s="98"/>
+      <c r="J42" s="96"/>
+      <c r="K42" s="96"/>
     </row>
     <row r="43" spans="1:12">
-      <c r="A43" s="145"/>
-      <c r="B43" s="96" t="s">
+      <c r="A43" s="142"/>
+      <c r="B43" s="94" t="s">
         <v>84</v>
       </c>
-      <c r="C43" s="97">
+      <c r="C43" s="95">
         <f t="shared" si="3"/>
         <v>83432</v>
       </c>
-      <c r="D43" s="97">
+      <c r="D43" s="95">
         <f t="shared" si="2"/>
         <v>83508</v>
       </c>
-      <c r="E43" s="97">
+      <c r="E43" s="95">
         <v>76</v>
       </c>
-      <c r="F43" s="148"/>
-      <c r="G43" s="148"/>
-      <c r="H43" s="147"/>
-      <c r="I43" s="147"/>
-      <c r="J43" s="98"/>
-      <c r="K43" s="98"/>
+      <c r="F43" s="145"/>
+      <c r="G43" s="145"/>
+      <c r="H43" s="144"/>
+      <c r="I43" s="144"/>
+      <c r="J43" s="96"/>
+      <c r="K43" s="96"/>
     </row>
     <row r="44" spans="1:12">
-      <c r="A44" s="145"/>
-      <c r="B44" s="96" t="s">
+      <c r="A44" s="142"/>
+      <c r="B44" s="94" t="s">
         <v>85</v>
       </c>
-      <c r="C44" s="97">
+      <c r="C44" s="95">
         <f t="shared" si="3"/>
         <v>83508</v>
       </c>
-      <c r="D44" s="97">
+      <c r="D44" s="95">
         <f t="shared" si="2"/>
         <v>83584</v>
       </c>
-      <c r="E44" s="97">
+      <c r="E44" s="95">
         <v>76</v>
       </c>
-      <c r="F44" s="148"/>
-      <c r="G44" s="148"/>
-      <c r="H44" s="147"/>
-      <c r="I44" s="147"/>
-      <c r="J44" s="98"/>
-      <c r="K44" s="98"/>
+      <c r="F44" s="145"/>
+      <c r="G44" s="145"/>
+      <c r="H44" s="144"/>
+      <c r="I44" s="144"/>
+      <c r="J44" s="96"/>
+      <c r="K44" s="96"/>
     </row>
     <row r="45" spans="1:12">
-      <c r="A45" s="145"/>
-      <c r="B45" s="96" t="s">
+      <c r="A45" s="142"/>
+      <c r="B45" s="94" t="s">
         <v>86</v>
       </c>
-      <c r="C45" s="97">
+      <c r="C45" s="95">
         <f t="shared" si="3"/>
         <v>83584</v>
       </c>
-      <c r="D45" s="97">
+      <c r="D45" s="95">
         <f t="shared" si="2"/>
         <v>83660</v>
       </c>
-      <c r="E45" s="97">
+      <c r="E45" s="95">
         <v>76</v>
       </c>
-      <c r="F45" s="148"/>
-      <c r="G45" s="148"/>
-      <c r="H45" s="147"/>
-      <c r="I45" s="147"/>
-      <c r="J45" s="98"/>
-      <c r="K45" s="98"/>
+      <c r="F45" s="145"/>
+      <c r="G45" s="145"/>
+      <c r="H45" s="144"/>
+      <c r="I45" s="144"/>
+      <c r="J45" s="96"/>
+      <c r="K45" s="96"/>
     </row>
     <row r="46" spans="1:12">
-      <c r="A46" s="145"/>
-      <c r="B46" s="96" t="s">
+      <c r="A46" s="142"/>
+      <c r="B46" s="94" t="s">
         <v>87</v>
       </c>
-      <c r="C46" s="97"/>
-      <c r="D46" s="97"/>
-      <c r="E46" s="97">
+      <c r="C46" s="95"/>
+      <c r="D46" s="95"/>
+      <c r="E46" s="95">
         <v>0</v>
       </c>
-      <c r="F46" s="148"/>
-      <c r="G46" s="148"/>
-      <c r="H46" s="147"/>
-      <c r="I46" s="147"/>
-      <c r="J46" s="98"/>
-      <c r="K46" s="98"/>
-      <c r="L46" s="117"/>
+      <c r="F46" s="145"/>
+      <c r="G46" s="145"/>
+      <c r="H46" s="144"/>
+      <c r="I46" s="144"/>
+      <c r="J46" s="96"/>
+      <c r="K46" s="96"/>
+      <c r="L46" s="115"/>
     </row>
     <row r="47" spans="1:12">
-      <c r="A47" s="142">
+      <c r="A47" s="139">
         <f>A42+7</f>
         <v>43748</v>
       </c>
-      <c r="B47" s="94" t="s">
+      <c r="B47" s="92" t="s">
         <v>83</v>
       </c>
-      <c r="C47" s="93"/>
-      <c r="D47" s="93"/>
-      <c r="E47" s="93">
+      <c r="C47" s="91"/>
+      <c r="D47" s="91"/>
+      <c r="E47" s="91">
         <v>0</v>
       </c>
-      <c r="F47" s="143">
+      <c r="F47" s="140">
         <f>SUM(E47:E51)</f>
         <v>304</v>
       </c>
-      <c r="G47" s="143">
+      <c r="G47" s="140">
         <f>G42+F47</f>
         <v>2964</v>
       </c>
-      <c r="H47" s="144">
+      <c r="H47" s="141">
         <f>F47*$I$2</f>
         <v>136.80000000000001</v>
       </c>
-      <c r="I47" s="144">
+      <c r="I47" s="141">
         <f>I42+H47</f>
         <v>1333.8</v>
       </c>
-      <c r="J47" s="95"/>
-      <c r="K47" s="95"/>
-      <c r="L47" s="117"/>
+      <c r="J47" s="93"/>
+      <c r="K47" s="93"/>
+      <c r="L47" s="115"/>
     </row>
     <row r="48" spans="1:12">
-      <c r="A48" s="142"/>
-      <c r="B48" s="94" t="s">
+      <c r="A48" s="139"/>
+      <c r="B48" s="92" t="s">
         <v>84</v>
       </c>
-      <c r="C48" s="93">
+      <c r="C48" s="91">
         <f>D45</f>
         <v>83660</v>
       </c>
-      <c r="D48" s="93">
+      <c r="D48" s="91">
         <f t="shared" si="2"/>
         <v>83736</v>
       </c>
-      <c r="E48" s="93">
+      <c r="E48" s="91">
         <v>76</v>
       </c>
-      <c r="F48" s="143"/>
-      <c r="G48" s="143"/>
-      <c r="H48" s="144"/>
-      <c r="I48" s="144"/>
-      <c r="J48" s="95"/>
-      <c r="K48" s="95"/>
+      <c r="F48" s="140"/>
+      <c r="G48" s="140"/>
+      <c r="H48" s="141"/>
+      <c r="I48" s="141"/>
+      <c r="J48" s="93"/>
+      <c r="K48" s="93"/>
     </row>
     <row r="49" spans="1:11">
-      <c r="A49" s="142"/>
-      <c r="B49" s="94" t="s">
+      <c r="A49" s="139"/>
+      <c r="B49" s="92" t="s">
         <v>85</v>
       </c>
-      <c r="C49" s="93">
+      <c r="C49" s="91">
         <f t="shared" si="3"/>
         <v>83736</v>
       </c>
-      <c r="D49" s="93">
+      <c r="D49" s="91">
         <f t="shared" si="2"/>
         <v>83812</v>
       </c>
-      <c r="E49" s="93">
+      <c r="E49" s="91">
         <v>76</v>
       </c>
-      <c r="F49" s="143"/>
-      <c r="G49" s="143"/>
-      <c r="H49" s="144"/>
-      <c r="I49" s="144"/>
-      <c r="J49" s="95"/>
-      <c r="K49" s="95"/>
+      <c r="F49" s="140"/>
+      <c r="G49" s="140"/>
+      <c r="H49" s="141"/>
+      <c r="I49" s="141"/>
+      <c r="J49" s="93"/>
+      <c r="K49" s="93"/>
     </row>
     <row r="50" spans="1:11">
-      <c r="A50" s="142"/>
-      <c r="B50" s="94" t="s">
+      <c r="A50" s="139"/>
+      <c r="B50" s="92" t="s">
         <v>86</v>
       </c>
-      <c r="C50" s="93">
+      <c r="C50" s="91">
         <f t="shared" si="3"/>
         <v>83812</v>
       </c>
-      <c r="D50" s="93">
+      <c r="D50" s="91">
         <f t="shared" si="2"/>
         <v>83888</v>
       </c>
-      <c r="E50" s="93">
+      <c r="E50" s="91">
         <v>76</v>
       </c>
-      <c r="F50" s="143"/>
-      <c r="G50" s="143"/>
-      <c r="H50" s="144"/>
-      <c r="I50" s="144"/>
-      <c r="J50" s="95"/>
-      <c r="K50" s="95"/>
+      <c r="F50" s="140"/>
+      <c r="G50" s="140"/>
+      <c r="H50" s="141"/>
+      <c r="I50" s="141"/>
+      <c r="J50" s="93"/>
+      <c r="K50" s="93"/>
     </row>
     <row r="51" spans="1:11">
-      <c r="A51" s="142"/>
-      <c r="B51" s="94" t="s">
+      <c r="A51" s="139"/>
+      <c r="B51" s="92" t="s">
         <v>87</v>
       </c>
-      <c r="C51" s="93">
+      <c r="C51" s="91">
         <f>D50</f>
         <v>83888</v>
       </c>
-      <c r="D51" s="93">
+      <c r="D51" s="91">
         <f>C51+E51</f>
         <v>83964</v>
       </c>
-      <c r="E51" s="93">
+      <c r="E51" s="91">
         <v>76</v>
       </c>
-      <c r="F51" s="143"/>
-      <c r="G51" s="143"/>
-      <c r="H51" s="144"/>
-      <c r="I51" s="144"/>
-      <c r="J51" s="95"/>
-      <c r="K51" s="95"/>
+      <c r="F51" s="140"/>
+      <c r="G51" s="140"/>
+      <c r="H51" s="141"/>
+      <c r="I51" s="141"/>
+      <c r="J51" s="93"/>
+      <c r="K51" s="93"/>
     </row>
     <row r="52" spans="1:11">
-      <c r="A52" s="145"/>
-      <c r="B52" s="96"/>
-      <c r="C52" s="97"/>
-      <c r="D52" s="97"/>
-      <c r="E52" s="97"/>
-      <c r="F52" s="148">
+      <c r="A52" s="142"/>
+      <c r="B52" s="94"/>
+      <c r="C52" s="95"/>
+      <c r="D52" s="95"/>
+      <c r="E52" s="95"/>
+      <c r="F52" s="145">
         <f>SUM(E52:E56)</f>
         <v>0</v>
       </c>
-      <c r="G52" s="148">
+      <c r="G52" s="145">
         <f>G47+F52</f>
         <v>2964</v>
       </c>
-      <c r="H52" s="147">
+      <c r="H52" s="144">
         <f>F52*$I$2</f>
         <v>0</v>
       </c>
-      <c r="I52" s="147">
+      <c r="I52" s="144">
         <f>I47+H52</f>
         <v>1333.8</v>
       </c>
-      <c r="J52" s="98"/>
-      <c r="K52" s="98"/>
+      <c r="J52" s="96"/>
+      <c r="K52" s="96"/>
     </row>
     <row r="53" spans="1:11">
-      <c r="A53" s="145"/>
-      <c r="B53" s="96"/>
-      <c r="C53" s="97"/>
-      <c r="D53" s="97"/>
-      <c r="E53" s="97"/>
-      <c r="F53" s="148"/>
-      <c r="G53" s="148"/>
-      <c r="H53" s="147"/>
-      <c r="I53" s="147"/>
-      <c r="J53" s="98"/>
-      <c r="K53" s="98"/>
+      <c r="A53" s="142"/>
+      <c r="B53" s="94"/>
+      <c r="C53" s="95"/>
+      <c r="D53" s="95"/>
+      <c r="E53" s="95"/>
+      <c r="F53" s="145"/>
+      <c r="G53" s="145"/>
+      <c r="H53" s="144"/>
+      <c r="I53" s="144"/>
+      <c r="J53" s="96"/>
+      <c r="K53" s="96"/>
     </row>
     <row r="54" spans="1:11">
-      <c r="A54" s="145"/>
-      <c r="B54" s="96"/>
-      <c r="C54" s="97"/>
-      <c r="D54" s="97"/>
-      <c r="E54" s="97"/>
-      <c r="F54" s="148"/>
-      <c r="G54" s="148"/>
-      <c r="H54" s="147"/>
-      <c r="I54" s="147"/>
-      <c r="J54" s="98"/>
-      <c r="K54" s="98"/>
+      <c r="A54" s="142"/>
+      <c r="B54" s="94"/>
+      <c r="C54" s="95"/>
+      <c r="D54" s="95"/>
+      <c r="E54" s="95"/>
+      <c r="F54" s="145"/>
+      <c r="G54" s="145"/>
+      <c r="H54" s="144"/>
+      <c r="I54" s="144"/>
+      <c r="J54" s="96"/>
+      <c r="K54" s="96"/>
     </row>
     <row r="55" spans="1:11">
-      <c r="A55" s="145"/>
-      <c r="B55" s="96"/>
-      <c r="C55" s="97"/>
-      <c r="D55" s="97"/>
-      <c r="E55" s="97"/>
-      <c r="F55" s="148"/>
-      <c r="G55" s="148"/>
-      <c r="H55" s="147"/>
-      <c r="I55" s="147"/>
-      <c r="J55" s="98"/>
-      <c r="K55" s="98"/>
+      <c r="A55" s="142"/>
+      <c r="B55" s="94"/>
+      <c r="C55" s="95"/>
+      <c r="D55" s="95"/>
+      <c r="E55" s="95"/>
+      <c r="F55" s="145"/>
+      <c r="G55" s="145"/>
+      <c r="H55" s="144"/>
+      <c r="I55" s="144"/>
+      <c r="J55" s="96"/>
+      <c r="K55" s="96"/>
     </row>
     <row r="56" spans="1:11">
-      <c r="A56" s="145"/>
-      <c r="B56" s="96"/>
-      <c r="C56" s="97"/>
-      <c r="D56" s="97"/>
-      <c r="E56" s="97"/>
-      <c r="F56" s="148"/>
-      <c r="G56" s="148"/>
-      <c r="H56" s="147"/>
-      <c r="I56" s="147"/>
-      <c r="J56" s="98"/>
-      <c r="K56" s="98"/>
+      <c r="A56" s="142"/>
+      <c r="B56" s="94"/>
+      <c r="C56" s="95"/>
+      <c r="D56" s="95"/>
+      <c r="E56" s="95"/>
+      <c r="F56" s="145"/>
+      <c r="G56" s="145"/>
+      <c r="H56" s="144"/>
+      <c r="I56" s="144"/>
+      <c r="J56" s="96"/>
+      <c r="K56" s="96"/>
     </row>
     <row r="57" spans="1:11">
-      <c r="A57" s="142"/>
-      <c r="B57" s="94"/>
-      <c r="C57" s="93"/>
-      <c r="D57" s="93"/>
-      <c r="E57" s="93"/>
-      <c r="F57" s="143">
+      <c r="A57" s="139"/>
+      <c r="B57" s="92"/>
+      <c r="C57" s="91"/>
+      <c r="D57" s="91"/>
+      <c r="E57" s="91"/>
+      <c r="F57" s="140">
         <f>SUM(E57:E61)</f>
         <v>0</v>
       </c>
-      <c r="G57" s="143">
+      <c r="G57" s="140">
         <f>G52+F57</f>
         <v>2964</v>
       </c>
-      <c r="H57" s="144">
+      <c r="H57" s="141">
         <f>F57*$I$2</f>
         <v>0</v>
       </c>
-      <c r="I57" s="144">
+      <c r="I57" s="141">
         <f>I52+H57</f>
         <v>1333.8</v>
       </c>
-      <c r="J57" s="95"/>
-      <c r="K57" s="95"/>
+      <c r="J57" s="93"/>
+      <c r="K57" s="93"/>
     </row>
     <row r="58" spans="1:11">
-      <c r="A58" s="142"/>
-      <c r="B58" s="94"/>
-      <c r="C58" s="93"/>
-      <c r="D58" s="93"/>
-      <c r="E58" s="93"/>
-      <c r="F58" s="143"/>
-      <c r="G58" s="143"/>
-      <c r="H58" s="144"/>
-      <c r="I58" s="144"/>
-      <c r="J58" s="95"/>
-      <c r="K58" s="95"/>
+      <c r="A58" s="139"/>
+      <c r="B58" s="92"/>
+      <c r="C58" s="91"/>
+      <c r="D58" s="91"/>
+      <c r="E58" s="91"/>
+      <c r="F58" s="140"/>
+      <c r="G58" s="140"/>
+      <c r="H58" s="141"/>
+      <c r="I58" s="141"/>
+      <c r="J58" s="93"/>
+      <c r="K58" s="93"/>
     </row>
     <row r="59" spans="1:11">
-      <c r="A59" s="142"/>
-      <c r="B59" s="94"/>
-      <c r="C59" s="93"/>
-      <c r="D59" s="93"/>
-      <c r="E59" s="93"/>
-      <c r="F59" s="143"/>
-      <c r="G59" s="143"/>
-      <c r="H59" s="144"/>
-      <c r="I59" s="144"/>
-      <c r="J59" s="95"/>
-      <c r="K59" s="95"/>
+      <c r="A59" s="139"/>
+      <c r="B59" s="92"/>
+      <c r="C59" s="91"/>
+      <c r="D59" s="91"/>
+      <c r="E59" s="91"/>
+      <c r="F59" s="140"/>
+      <c r="G59" s="140"/>
+      <c r="H59" s="141"/>
+      <c r="I59" s="141"/>
+      <c r="J59" s="93"/>
+      <c r="K59" s="93"/>
     </row>
     <row r="60" spans="1:11">
-      <c r="A60" s="142"/>
-      <c r="B60" s="94"/>
-      <c r="C60" s="93"/>
-      <c r="D60" s="93"/>
-      <c r="E60" s="93"/>
-      <c r="F60" s="143"/>
-      <c r="G60" s="143"/>
-      <c r="H60" s="144"/>
-      <c r="I60" s="144"/>
-      <c r="J60" s="95"/>
-      <c r="K60" s="95"/>
+      <c r="A60" s="139"/>
+      <c r="B60" s="92"/>
+      <c r="C60" s="91"/>
+      <c r="D60" s="91"/>
+      <c r="E60" s="91"/>
+      <c r="F60" s="140"/>
+      <c r="G60" s="140"/>
+      <c r="H60" s="141"/>
+      <c r="I60" s="141"/>
+      <c r="J60" s="93"/>
+      <c r="K60" s="93"/>
     </row>
     <row r="61" spans="1:11">
-      <c r="A61" s="142"/>
-      <c r="B61" s="94"/>
-      <c r="C61" s="93"/>
-      <c r="D61" s="93"/>
-      <c r="E61" s="93"/>
-      <c r="F61" s="143"/>
-      <c r="G61" s="143"/>
-      <c r="H61" s="144"/>
-      <c r="I61" s="144"/>
-      <c r="J61" s="95"/>
-      <c r="K61" s="95"/>
+      <c r="A61" s="139"/>
+      <c r="B61" s="92"/>
+      <c r="C61" s="91"/>
+      <c r="D61" s="91"/>
+      <c r="E61" s="91"/>
+      <c r="F61" s="140"/>
+      <c r="G61" s="140"/>
+      <c r="H61" s="141"/>
+      <c r="I61" s="141"/>
+      <c r="J61" s="93"/>
+      <c r="K61" s="93"/>
     </row>
     <row r="62" spans="1:11">
-      <c r="A62" s="145"/>
-      <c r="B62" s="96"/>
-      <c r="C62" s="97"/>
-      <c r="D62" s="97"/>
-      <c r="E62" s="97"/>
-      <c r="F62" s="148">
+      <c r="A62" s="142"/>
+      <c r="B62" s="94"/>
+      <c r="C62" s="95"/>
+      <c r="D62" s="95"/>
+      <c r="E62" s="95"/>
+      <c r="F62" s="145">
         <f>SUM(E62:E66)</f>
         <v>0</v>
       </c>
-      <c r="G62" s="148">
+      <c r="G62" s="145">
         <f>G57+F62</f>
         <v>2964</v>
       </c>
-      <c r="H62" s="147">
+      <c r="H62" s="144">
         <f>F62*$I$2</f>
         <v>0</v>
       </c>
-      <c r="I62" s="147">
+      <c r="I62" s="144">
         <f>I57+H62</f>
         <v>1333.8</v>
       </c>
-      <c r="J62" s="98"/>
-      <c r="K62" s="98"/>
+      <c r="J62" s="96"/>
+      <c r="K62" s="96"/>
     </row>
     <row r="63" spans="1:11">
-      <c r="A63" s="145"/>
-      <c r="B63" s="96"/>
-      <c r="C63" s="97"/>
-      <c r="D63" s="97"/>
-      <c r="E63" s="97"/>
-      <c r="F63" s="148"/>
-      <c r="G63" s="148"/>
-      <c r="H63" s="147"/>
-      <c r="I63" s="147"/>
-      <c r="J63" s="98"/>
-      <c r="K63" s="98"/>
+      <c r="A63" s="142"/>
+      <c r="B63" s="94"/>
+      <c r="C63" s="95"/>
+      <c r="D63" s="95"/>
+      <c r="E63" s="95"/>
+      <c r="F63" s="145"/>
+      <c r="G63" s="145"/>
+      <c r="H63" s="144"/>
+      <c r="I63" s="144"/>
+      <c r="J63" s="96"/>
+      <c r="K63" s="96"/>
     </row>
     <row r="64" spans="1:11">
-      <c r="A64" s="145"/>
-      <c r="B64" s="96"/>
-      <c r="C64" s="97"/>
-      <c r="D64" s="97"/>
-      <c r="E64" s="97"/>
-      <c r="F64" s="148"/>
-      <c r="G64" s="148"/>
-      <c r="H64" s="147"/>
-      <c r="I64" s="147"/>
-      <c r="J64" s="98"/>
-      <c r="K64" s="98"/>
+      <c r="A64" s="142"/>
+      <c r="B64" s="94"/>
+      <c r="C64" s="95"/>
+      <c r="D64" s="95"/>
+      <c r="E64" s="95"/>
+      <c r="F64" s="145"/>
+      <c r="G64" s="145"/>
+      <c r="H64" s="144"/>
+      <c r="I64" s="144"/>
+      <c r="J64" s="96"/>
+      <c r="K64" s="96"/>
     </row>
     <row r="65" spans="1:11">
-      <c r="A65" s="145"/>
-      <c r="B65" s="96"/>
-      <c r="C65" s="97"/>
-      <c r="D65" s="97"/>
-      <c r="E65" s="97"/>
-      <c r="F65" s="148"/>
-      <c r="G65" s="148"/>
-      <c r="H65" s="147"/>
-      <c r="I65" s="147"/>
-      <c r="J65" s="98"/>
-      <c r="K65" s="98"/>
+      <c r="A65" s="142"/>
+      <c r="B65" s="94"/>
+      <c r="C65" s="95"/>
+      <c r="D65" s="95"/>
+      <c r="E65" s="95"/>
+      <c r="F65" s="145"/>
+      <c r="G65" s="145"/>
+      <c r="H65" s="144"/>
+      <c r="I65" s="144"/>
+      <c r="J65" s="96"/>
+      <c r="K65" s="96"/>
     </row>
     <row r="66" spans="1:11">
-      <c r="A66" s="145"/>
-      <c r="B66" s="96"/>
-      <c r="C66" s="97"/>
-      <c r="D66" s="97"/>
-      <c r="E66" s="97"/>
-      <c r="F66" s="148"/>
-      <c r="G66" s="148"/>
-      <c r="H66" s="147"/>
-      <c r="I66" s="147"/>
-      <c r="J66" s="98"/>
-      <c r="K66" s="98"/>
+      <c r="A66" s="142"/>
+      <c r="B66" s="94"/>
+      <c r="C66" s="95"/>
+      <c r="D66" s="95"/>
+      <c r="E66" s="95"/>
+      <c r="F66" s="145"/>
+      <c r="G66" s="145"/>
+      <c r="H66" s="144"/>
+      <c r="I66" s="144"/>
+      <c r="J66" s="96"/>
+      <c r="K66" s="96"/>
     </row>
   </sheetData>
   <mergeCells count="61">

</xml_diff>

<commit_message>
Added constant summary headers
</commit_message>
<xml_diff>
--- a/Lava3.TestFiles/TestFiles/Test.xlsx
+++ b/Lava3.TestFiles/TestFiles/Test.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="510" yWindow="585" windowWidth="15555" windowHeight="13155" tabRatio="554" activeTab="2"/>
+    <workbookView xWindow="510" yWindow="585" windowWidth="15555" windowHeight="13155" tabRatio="554"/>
   </bookViews>
   <sheets>
     <sheet name="Annual Summary" sheetId="2" r:id="rId1"/>
@@ -3543,9 +3543,9 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:AB75"/>
   <sheetViews>
-    <sheetView zoomScale="80" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="80" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D38" sqref="D38"/>
+      <selection pane="bottomLeft" activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.625" defaultRowHeight="12"/>
@@ -5067,7 +5067,7 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:J61"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="D26" sqref="D26"/>
     </sheetView>

</xml_diff>